<commit_message>
Added Made easy test analysis
</commit_message>
<xml_diff>
--- a/My Marks Tracker.xlsx
+++ b/My Marks Tracker.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GATE 2022 &amp; 2023\My Progress trackers &amp; Journey - In Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C5FEC46-12A5-4C44-85AB-84828F800569}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B82A483C-CB59-4D19-AE8C-F7CC55786BB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3209D17C-0F5C-4895-BA2D-FBE4C1879A87}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="55">
   <si>
     <t>Test Name</t>
   </si>
@@ -194,6 +194,9 @@
   </si>
   <si>
     <t>Diff with Topper</t>
+  </si>
+  <si>
+    <t>#Percentile</t>
   </si>
 </sst>
 </file>
@@ -540,7 +543,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -692,34 +695,6 @@
     <xf numFmtId="0" fontId="0" fillId="13" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="14" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -761,12 +736,42 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="108">
+  <dxfs count="8">
     <dxf>
       <fill>
         <patternFill>
@@ -808,944 +813,6 @@
       <fill>
         <patternFill>
           <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2051,6 +1118,9 @@
                 </c:pt>
                 <c:pt idx="23">
                   <c:v>61.7</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>66.36</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2474,6 +1544,9 @@
                 <c:pt idx="23">
                   <c:v>71.430000000000007</c:v>
                 </c:pt>
+                <c:pt idx="24">
+                  <c:v>71.430000000000007</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2796,7 +1869,7 @@
                   <c:v>0.32999999999999829</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0</c:v>
+                  <c:v>8.6599999999999966</c:v>
                 </c:pt>
                 <c:pt idx="25">
                   <c:v>0</c:v>
@@ -2996,6 +2069,406 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:areaChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$R$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>#Percentile</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$R$2:$R$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="40"/>
+                <c:pt idx="0">
+                  <c:v>41.791044776119399</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43.781094527363187</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>76.966747769667478</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>68.346111719605702</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>74.089635854341736</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>62.477231329690341</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>60.098522167487687</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>74.698795180722882</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>79.343863912515189</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>64.772727272727266</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>67.963386727688786</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>71.890547263681597</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>99.861999999999995</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>99.831000000000003</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>99.866666666666674</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>70.337078651685388</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>97.718631178707227</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>84.277456647398836</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>85.593220338983059</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>98.319327731092429</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>89.772727272727266</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>90.384615384615387</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>92.307692307692307</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-964A-42BC-B88F-B2E79615D280}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="930156304"/>
+        <c:axId val="930143824"/>
+      </c:areaChart>
+      <c:catAx>
+        <c:axId val="930156304"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="95000"/>
+                <a:alpha val="54000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="930143824"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="930143824"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="930156304"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="withinLinear" id="15">
   <a:schemeClr val="accent2"/>
@@ -3082,6 +2555,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="202">
   <cs:axisTitle>
@@ -4612,6 +4125,502 @@
         <a:noFill/>
       </a:ln>
     </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="283">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="34925" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -4721,6 +4730,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>103093</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>161365</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>67235</xdr:colOff>
+      <xdr:row>76</xdr:row>
+      <xdr:rowOff>35860</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{79CD4FFD-89BD-82A9-1D70-80C1221BCEB8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -5028,13 +5073,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E08F6CAB-EED7-4179-B275-45A8F5F85EF1}">
   <dimension ref="A1:T41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N26" sqref="N26"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q16" sqref="Q16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.21875" customWidth="1"/>
     <col min="4" max="4" width="41.33203125" style="1" customWidth="1"/>
     <col min="5" max="5" width="7.5546875" style="2" customWidth="1"/>
@@ -5046,7 +5092,7 @@
     <col min="11" max="11" width="12.6640625" style="5" customWidth="1"/>
     <col min="12" max="12" width="8.88671875" style="6"/>
     <col min="13" max="13" width="17.77734375" style="9" customWidth="1"/>
-    <col min="14" max="14" width="8.88671875" style="89"/>
+    <col min="14" max="14" width="8.88671875" style="79"/>
     <col min="15" max="15" width="10.5546875" style="10" customWidth="1"/>
     <col min="16" max="17" width="8.88671875" style="7"/>
     <col min="18" max="18" width="11.77734375" style="3" bestFit="1" customWidth="1"/>
@@ -5060,10 +5106,10 @@
       <c r="B1" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="71" t="s">
+      <c r="C1" s="85" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="71"/>
+      <c r="D1" s="85"/>
       <c r="E1" s="35" t="s">
         <v>3</v>
       </c>
@@ -5091,7 +5137,7 @@
       <c r="M1" s="42" t="s">
         <v>23</v>
       </c>
-      <c r="N1" s="83" t="s">
+      <c r="N1" s="73" t="s">
         <v>14</v>
       </c>
       <c r="O1" s="43" t="s">
@@ -5100,11 +5146,13 @@
       <c r="P1" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="Q1" s="76" t="s">
+      <c r="Q1" s="66" t="s">
         <v>22</v>
       </c>
-      <c r="R1" s="3"/>
-      <c r="T1" s="75" t="s">
+      <c r="R1" s="91" t="s">
+        <v>54</v>
+      </c>
+      <c r="T1" s="65" t="s">
         <v>53</v>
       </c>
     </row>
@@ -5113,10 +5161,10 @@
       <c r="B2" s="57">
         <v>1</v>
       </c>
-      <c r="C2" s="72" t="s">
+      <c r="C2" s="86" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="72"/>
+      <c r="D2" s="86"/>
       <c r="E2" s="58">
         <v>41</v>
       </c>
@@ -5144,7 +5192,7 @@
       <c r="M2" s="58">
         <v>39.869999999999997</v>
       </c>
-      <c r="N2" s="84">
+      <c r="N2" s="74">
         <v>86.34</v>
       </c>
       <c r="O2" s="58">
@@ -5153,7 +5201,7 @@
       <c r="P2" s="58">
         <v>157</v>
       </c>
-      <c r="Q2" s="77">
+      <c r="Q2" s="67">
         <v>268</v>
       </c>
       <c r="R2" s="3">
@@ -5170,10 +5218,10 @@
       <c r="B3" s="60">
         <v>2</v>
       </c>
-      <c r="C3" s="69" t="s">
+      <c r="C3" s="84" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="69"/>
+      <c r="D3" s="84"/>
       <c r="E3" s="61">
         <v>40</v>
       </c>
@@ -5201,7 +5249,7 @@
       <c r="M3" s="61">
         <v>39.18</v>
       </c>
-      <c r="N3" s="85">
+      <c r="N3" s="75">
         <v>84.69</v>
       </c>
       <c r="O3" s="61">
@@ -5210,7 +5258,7 @@
       <c r="P3" s="61">
         <v>114</v>
       </c>
-      <c r="Q3" s="78">
+      <c r="Q3" s="68">
         <v>201</v>
       </c>
       <c r="R3" s="3">
@@ -5218,7 +5266,7 @@
         <v>43.781094527363187</v>
       </c>
       <c r="T3" s="3">
-        <f t="shared" ref="T3:T35" si="1">N3-L3</f>
+        <f>N3-L3</f>
         <v>46.989999999999995</v>
       </c>
     </row>
@@ -5227,10 +5275,10 @@
       <c r="B4" s="60">
         <v>3</v>
       </c>
-      <c r="C4" s="69" t="s">
+      <c r="C4" s="84" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="69"/>
+      <c r="D4" s="84"/>
       <c r="E4" s="61">
         <v>51</v>
       </c>
@@ -5258,7 +5306,7 @@
       <c r="M4" s="61">
         <v>33.14</v>
       </c>
-      <c r="N4" s="85">
+      <c r="N4" s="75">
         <v>81.7</v>
       </c>
       <c r="O4" s="61">
@@ -5267,7 +5315,7 @@
       <c r="P4" s="61">
         <v>285</v>
       </c>
-      <c r="Q4" s="78">
+      <c r="Q4" s="68">
         <v>1233</v>
       </c>
       <c r="R4" s="3">
@@ -5275,7 +5323,7 @@
         <v>76.966747769667478</v>
       </c>
       <c r="T4" s="3">
-        <f t="shared" si="1"/>
+        <f>N4-L4</f>
         <v>34.32</v>
       </c>
     </row>
@@ -5284,10 +5332,10 @@
       <c r="B5" s="60">
         <v>4</v>
       </c>
-      <c r="C5" s="69" t="s">
+      <c r="C5" s="84" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="69"/>
+      <c r="D5" s="84"/>
       <c r="E5" s="61">
         <v>51</v>
       </c>
@@ -5311,18 +5359,18 @@
         <v>52.33</v>
       </c>
       <c r="M5" s="61"/>
-      <c r="N5" s="85">
+      <c r="N5" s="75">
         <v>91</v>
       </c>
       <c r="O5" s="61"/>
       <c r="P5" s="61"/>
-      <c r="Q5" s="78"/>
+      <c r="Q5" s="68"/>
       <c r="R5" s="3" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="T5" s="3">
-        <f t="shared" si="1"/>
+        <f>N5-L5</f>
         <v>38.67</v>
       </c>
     </row>
@@ -5331,10 +5379,10 @@
       <c r="B6" s="60">
         <v>5</v>
       </c>
-      <c r="C6" s="69" t="s">
+      <c r="C6" s="84" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="69"/>
+      <c r="D6" s="84"/>
       <c r="E6" s="61">
         <v>47</v>
       </c>
@@ -5362,7 +5410,7 @@
       <c r="M6" s="61">
         <v>39.799999999999997</v>
       </c>
-      <c r="N6" s="85">
+      <c r="N6" s="75">
         <v>87.36</v>
       </c>
       <c r="O6" s="61">
@@ -5371,7 +5419,7 @@
       <c r="P6" s="61">
         <v>290</v>
       </c>
-      <c r="Q6" s="78">
+      <c r="Q6" s="68">
         <v>913</v>
       </c>
       <c r="R6" s="3">
@@ -5379,7 +5427,7 @@
         <v>68.346111719605702</v>
       </c>
       <c r="T6" s="3">
-        <f t="shared" si="1"/>
+        <f>N6-L6</f>
         <v>38.01</v>
       </c>
     </row>
@@ -5388,10 +5436,10 @@
       <c r="B7" s="60">
         <v>6</v>
       </c>
-      <c r="C7" s="69" t="s">
+      <c r="C7" s="84" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="69"/>
+      <c r="D7" s="84"/>
       <c r="E7" s="61">
         <v>51</v>
       </c>
@@ -5419,7 +5467,7 @@
       <c r="M7" s="61">
         <v>37.15</v>
       </c>
-      <c r="N7" s="85">
+      <c r="N7" s="75">
         <v>79.67</v>
       </c>
       <c r="O7" s="61">
@@ -5428,7 +5476,7 @@
       <c r="P7" s="61">
         <v>186</v>
       </c>
-      <c r="Q7" s="78">
+      <c r="Q7" s="68">
         <v>714</v>
       </c>
       <c r="R7" s="3">
@@ -5436,7 +5484,7 @@
         <v>74.089635854341736</v>
       </c>
       <c r="T7" s="3">
-        <f t="shared" si="1"/>
+        <f>N7-L7</f>
         <v>31.97</v>
       </c>
     </row>
@@ -5445,10 +5493,10 @@
       <c r="B8" s="60">
         <v>7</v>
       </c>
-      <c r="C8" s="69" t="s">
+      <c r="C8" s="84" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="69"/>
+      <c r="D8" s="84"/>
       <c r="E8" s="61">
         <v>52</v>
       </c>
@@ -5476,7 +5524,7 @@
       <c r="M8" s="61">
         <v>44.06</v>
       </c>
-      <c r="N8" s="85">
+      <c r="N8" s="75">
         <v>88.02</v>
       </c>
       <c r="O8" s="61">
@@ -5485,7 +5533,7 @@
       <c r="P8" s="61">
         <v>207</v>
       </c>
-      <c r="Q8" s="78">
+      <c r="Q8" s="68">
         <v>549</v>
       </c>
       <c r="R8" s="3">
@@ -5493,7 +5541,7 @@
         <v>62.477231329690341</v>
       </c>
       <c r="T8" s="3">
-        <f t="shared" si="1"/>
+        <f>N8-L8</f>
         <v>36.309999999999995</v>
       </c>
     </row>
@@ -5502,10 +5550,10 @@
       <c r="B9" s="60">
         <v>8</v>
       </c>
-      <c r="C9" s="69" t="s">
+      <c r="C9" s="84" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="69"/>
+      <c r="D9" s="84"/>
       <c r="E9" s="61">
         <v>55</v>
       </c>
@@ -5533,7 +5581,7 @@
       <c r="M9" s="61">
         <v>39.200000000000003</v>
       </c>
-      <c r="N9" s="85">
+      <c r="N9" s="75">
         <v>81.680000000000007</v>
       </c>
       <c r="O9" s="61">
@@ -5542,7 +5590,7 @@
       <c r="P9" s="61">
         <v>82</v>
       </c>
-      <c r="Q9" s="78">
+      <c r="Q9" s="68">
         <v>203</v>
       </c>
       <c r="R9" s="3">
@@ -5550,7 +5598,7 @@
         <v>60.098522167487687</v>
       </c>
       <c r="T9" s="3">
-        <f t="shared" si="1"/>
+        <f>N9-L9</f>
         <v>35.660000000000004</v>
       </c>
     </row>
@@ -5559,10 +5607,10 @@
       <c r="B10" s="60">
         <v>9</v>
       </c>
-      <c r="C10" s="69" t="s">
+      <c r="C10" s="84" t="s">
         <v>26</v>
       </c>
-      <c r="D10" s="69"/>
+      <c r="D10" s="84"/>
       <c r="E10" s="61">
         <v>58</v>
       </c>
@@ -5590,7 +5638,7 @@
       <c r="M10" s="61">
         <v>42.88</v>
       </c>
-      <c r="N10" s="85">
+      <c r="N10" s="75">
         <v>86.02</v>
       </c>
       <c r="O10" s="61">
@@ -5599,7 +5647,7 @@
       <c r="P10" s="61">
         <v>43</v>
       </c>
-      <c r="Q10" s="78">
+      <c r="Q10" s="68">
         <v>166</v>
       </c>
       <c r="R10" s="3">
@@ -5607,7 +5655,7 @@
         <v>74.698795180722882</v>
       </c>
       <c r="T10" s="3">
-        <f t="shared" si="1"/>
+        <f>N10-L10</f>
         <v>26.299999999999997</v>
       </c>
     </row>
@@ -5616,10 +5664,10 @@
       <c r="B11" s="60">
         <v>10</v>
       </c>
-      <c r="C11" s="69" t="s">
+      <c r="C11" s="84" t="s">
         <v>27</v>
       </c>
-      <c r="D11" s="69"/>
+      <c r="D11" s="84"/>
       <c r="E11" s="61">
         <v>60</v>
       </c>
@@ -5647,7 +5695,7 @@
       <c r="M11" s="61">
         <v>43.61</v>
       </c>
-      <c r="N11" s="85">
+      <c r="N11" s="75">
         <v>83.02</v>
       </c>
       <c r="O11" s="61">
@@ -5656,7 +5704,7 @@
       <c r="P11" s="61">
         <v>171</v>
       </c>
-      <c r="Q11" s="78">
+      <c r="Q11" s="68">
         <v>823</v>
       </c>
       <c r="R11" s="3">
@@ -5664,7 +5712,7 @@
         <v>79.343863912515189</v>
       </c>
       <c r="T11" s="3">
-        <f t="shared" si="1"/>
+        <f>N11-L11</f>
         <v>25.639999999999993</v>
       </c>
     </row>
@@ -5673,10 +5721,10 @@
       <c r="B12" s="60">
         <v>11</v>
       </c>
-      <c r="C12" s="69" t="s">
+      <c r="C12" s="84" t="s">
         <v>28</v>
       </c>
-      <c r="D12" s="69"/>
+      <c r="D12" s="84"/>
       <c r="E12" s="61">
         <v>56</v>
       </c>
@@ -5704,7 +5752,7 @@
       <c r="M12" s="61">
         <v>50.53</v>
       </c>
-      <c r="N12" s="85">
+      <c r="N12" s="75">
         <v>90</v>
       </c>
       <c r="O12" s="61">
@@ -5713,7 +5761,7 @@
       <c r="P12" s="61">
         <v>218</v>
       </c>
-      <c r="Q12" s="78">
+      <c r="Q12" s="68">
         <v>616</v>
       </c>
       <c r="R12" s="3">
@@ -5721,7 +5769,7 @@
         <v>64.772727272727266</v>
       </c>
       <c r="T12" s="3">
-        <f t="shared" si="1"/>
+        <f>N12-L12</f>
         <v>30.310000000000002</v>
       </c>
     </row>
@@ -5730,10 +5778,10 @@
       <c r="B13" s="60">
         <v>12</v>
       </c>
-      <c r="C13" s="69" t="s">
+      <c r="C13" s="84" t="s">
         <v>29</v>
       </c>
-      <c r="D13" s="69"/>
+      <c r="D13" s="84"/>
       <c r="E13" s="61">
         <v>56</v>
       </c>
@@ -5761,7 +5809,7 @@
       <c r="M13" s="61">
         <v>52.6</v>
       </c>
-      <c r="N13" s="85">
+      <c r="N13" s="75">
         <v>89.34</v>
       </c>
       <c r="O13" s="61">
@@ -5770,7 +5818,7 @@
       <c r="P13" s="61">
         <v>141</v>
       </c>
-      <c r="Q13" s="78">
+      <c r="Q13" s="68">
         <v>437</v>
       </c>
       <c r="R13" s="3">
@@ -5778,7 +5826,7 @@
         <v>67.963386727688786</v>
       </c>
       <c r="T13" s="3">
-        <f t="shared" si="1"/>
+        <f>N13-L13</f>
         <v>24.64</v>
       </c>
     </row>
@@ -5787,10 +5835,10 @@
       <c r="B14" s="60">
         <v>13</v>
       </c>
-      <c r="C14" s="69" t="s">
+      <c r="C14" s="84" t="s">
         <v>30</v>
       </c>
-      <c r="D14" s="69"/>
+      <c r="D14" s="84"/>
       <c r="E14" s="61">
         <v>56</v>
       </c>
@@ -5818,7 +5866,7 @@
       <c r="M14" s="61">
         <v>46.4</v>
       </c>
-      <c r="N14" s="85">
+      <c r="N14" s="75">
         <v>84.35</v>
       </c>
       <c r="O14" s="61">
@@ -5827,7 +5875,7 @@
       <c r="P14" s="61">
         <v>114</v>
       </c>
-      <c r="Q14" s="78">
+      <c r="Q14" s="68">
         <v>402</v>
       </c>
       <c r="R14" s="3">
@@ -5835,7 +5883,7 @@
         <v>71.890547263681597</v>
       </c>
       <c r="T14" s="3">
-        <f t="shared" si="1"/>
+        <f>N14-L14</f>
         <v>23.989999999999995</v>
       </c>
     </row>
@@ -5844,10 +5892,10 @@
       <c r="B15" s="60">
         <v>14</v>
       </c>
-      <c r="C15" s="69" t="s">
+      <c r="C15" s="84" t="s">
         <v>31</v>
       </c>
-      <c r="D15" s="69"/>
+      <c r="D15" s="84"/>
       <c r="E15" s="61">
         <v>50</v>
       </c>
@@ -5873,14 +5921,14 @@
       <c r="M15" s="61">
         <v>40.450000000000003</v>
       </c>
-      <c r="N15" s="85">
+      <c r="N15" s="75">
         <v>78.81</v>
       </c>
       <c r="O15" s="61"/>
       <c r="P15" s="61">
         <v>139</v>
       </c>
-      <c r="Q15" s="78">
+      <c r="Q15" s="68">
         <v>100000</v>
       </c>
       <c r="R15" s="3">
@@ -5888,7 +5936,7 @@
         <v>99.861999999999995</v>
       </c>
       <c r="T15" s="3">
-        <f t="shared" si="1"/>
+        <f>N15-L15</f>
         <v>16.810000000000002</v>
       </c>
     </row>
@@ -5897,10 +5945,10 @@
       <c r="B16" s="60">
         <v>15</v>
       </c>
-      <c r="C16" s="69" t="s">
+      <c r="C16" s="84" t="s">
         <v>32</v>
       </c>
-      <c r="D16" s="69"/>
+      <c r="D16" s="84"/>
       <c r="E16" s="61">
         <v>56</v>
       </c>
@@ -5926,14 +5974,14 @@
       <c r="M16" s="61">
         <v>47.81</v>
       </c>
-      <c r="N16" s="85">
+      <c r="N16" s="75">
         <v>83.09</v>
       </c>
       <c r="O16" s="61"/>
       <c r="P16" s="61">
         <v>170</v>
       </c>
-      <c r="Q16" s="78">
+      <c r="Q16" s="68">
         <v>100000</v>
       </c>
       <c r="R16" s="3">
@@ -5941,7 +5989,7 @@
         <v>99.831000000000003</v>
       </c>
       <c r="T16" s="3">
-        <f t="shared" si="1"/>
+        <f>N16-L16</f>
         <v>13.430000000000007</v>
       </c>
     </row>
@@ -5950,10 +5998,10 @@
       <c r="B17" s="60">
         <v>16</v>
       </c>
-      <c r="C17" s="69" t="s">
+      <c r="C17" s="84" t="s">
         <v>33</v>
       </c>
-      <c r="D17" s="69"/>
+      <c r="D17" s="84"/>
       <c r="E17" s="61">
         <v>53</v>
       </c>
@@ -5979,14 +6027,14 @@
       <c r="M17" s="61">
         <v>43.84</v>
       </c>
-      <c r="N17" s="85">
+      <c r="N17" s="75">
         <v>82.46</v>
       </c>
       <c r="O17" s="61"/>
       <c r="P17" s="61">
         <v>201</v>
       </c>
-      <c r="Q17" s="78">
+      <c r="Q17" s="68">
         <v>150000</v>
       </c>
       <c r="R17" s="3">
@@ -5994,7 +6042,7 @@
         <v>99.866666666666674</v>
       </c>
       <c r="T17" s="3">
-        <f t="shared" si="1"/>
+        <f>N17-L17</f>
         <v>20.129999999999995</v>
       </c>
     </row>
@@ -6003,10 +6051,10 @@
       <c r="B18" s="60">
         <v>17</v>
       </c>
-      <c r="C18" s="69" t="s">
+      <c r="C18" s="84" t="s">
         <v>34</v>
       </c>
-      <c r="D18" s="69"/>
+      <c r="D18" s="84"/>
       <c r="E18" s="61">
         <v>58</v>
       </c>
@@ -6034,7 +6082,7 @@
       <c r="M18" s="61">
         <v>48.22</v>
       </c>
-      <c r="N18" s="85">
+      <c r="N18" s="75">
         <v>88.68</v>
       </c>
       <c r="O18" s="61">
@@ -6043,7 +6091,7 @@
       <c r="P18" s="61">
         <v>397</v>
       </c>
-      <c r="Q18" s="78">
+      <c r="Q18" s="68">
         <v>1335</v>
       </c>
       <c r="R18" s="3">
@@ -6051,7 +6099,7 @@
         <v>70.337078651685388</v>
       </c>
       <c r="T18" s="3">
-        <f t="shared" si="1"/>
+        <f>N18-L18</f>
         <v>29.650000000000006</v>
       </c>
     </row>
@@ -6060,10 +6108,10 @@
       <c r="B19" s="60">
         <v>18</v>
       </c>
-      <c r="C19" s="69" t="s">
+      <c r="C19" s="84" t="s">
         <v>35</v>
       </c>
-      <c r="D19" s="69"/>
+      <c r="D19" s="84"/>
       <c r="E19" s="61">
         <v>60</v>
       </c>
@@ -6091,7 +6139,7 @@
       <c r="M19" s="61">
         <v>49.92</v>
       </c>
-      <c r="N19" s="85">
+      <c r="N19" s="75">
         <v>86.68</v>
       </c>
       <c r="O19" s="61">
@@ -6100,7 +6148,7 @@
       <c r="P19" s="61">
         <v>31</v>
       </c>
-      <c r="Q19" s="78">
+      <c r="Q19" s="68">
         <v>1315</v>
       </c>
       <c r="R19" s="3">
@@ -6108,7 +6156,7 @@
         <v>97.718631178707227</v>
       </c>
       <c r="T19" s="3">
-        <f t="shared" si="1"/>
+        <f>N19-L19</f>
         <v>9</v>
       </c>
     </row>
@@ -6117,10 +6165,10 @@
       <c r="B20" s="60">
         <v>19</v>
       </c>
-      <c r="C20" s="69" t="s">
+      <c r="C20" s="84" t="s">
         <v>36</v>
       </c>
-      <c r="D20" s="69"/>
+      <c r="D20" s="84"/>
       <c r="E20" s="61">
         <v>59</v>
       </c>
@@ -6148,7 +6196,7 @@
       <c r="M20" s="61">
         <v>46.71</v>
       </c>
-      <c r="N20" s="85">
+      <c r="N20" s="75">
         <v>83</v>
       </c>
       <c r="O20" s="61">
@@ -6157,7 +6205,7 @@
       <c r="P20" s="61">
         <v>137</v>
       </c>
-      <c r="Q20" s="78">
+      <c r="Q20" s="68">
         <v>865</v>
       </c>
       <c r="R20" s="3">
@@ -6165,7 +6213,7 @@
         <v>84.277456647398836</v>
       </c>
       <c r="T20" s="3">
-        <f t="shared" si="1"/>
+        <f>N20-L20</f>
         <v>18.64</v>
       </c>
     </row>
@@ -6174,10 +6222,10 @@
       <c r="B21" s="63">
         <v>20</v>
       </c>
-      <c r="C21" s="73" t="s">
+      <c r="C21" s="87" t="s">
         <v>37</v>
       </c>
-      <c r="D21" s="73"/>
+      <c r="D21" s="87"/>
       <c r="E21" s="64">
         <v>56</v>
       </c>
@@ -6205,7 +6253,7 @@
       <c r="M21" s="64">
         <v>41.19</v>
       </c>
-      <c r="N21" s="86">
+      <c r="N21" s="76">
         <v>82.02</v>
       </c>
       <c r="O21" s="64">
@@ -6214,7 +6262,7 @@
       <c r="P21" s="64">
         <v>120</v>
       </c>
-      <c r="Q21" s="79">
+      <c r="Q21" s="69">
         <v>826</v>
       </c>
       <c r="R21" s="3">
@@ -6222,7 +6270,7 @@
         <v>85.593220338983059</v>
       </c>
       <c r="T21" s="3">
-        <f t="shared" si="1"/>
+        <f>N21-L21</f>
         <v>21.319999999999993</v>
       </c>
     </row>
@@ -6233,10 +6281,10 @@
       <c r="B22" s="45">
         <v>21</v>
       </c>
-      <c r="C22" s="65" t="s">
+      <c r="C22" s="88" t="s">
         <v>38</v>
       </c>
-      <c r="D22" s="66"/>
+      <c r="D22" s="89"/>
       <c r="E22" s="46">
         <v>57</v>
       </c>
@@ -6264,7 +6312,7 @@
       <c r="M22" s="54">
         <v>9.25</v>
       </c>
-      <c r="N22" s="87">
+      <c r="N22" s="77">
         <v>76.36</v>
       </c>
       <c r="O22" s="55">
@@ -6273,18 +6321,18 @@
       <c r="P22" s="50">
         <v>11</v>
       </c>
-      <c r="Q22" s="80">
+      <c r="Q22" s="70">
         <v>595</v>
       </c>
       <c r="R22" s="3">
-        <f t="shared" ref="R22:R30" si="2" xml:space="preserve"> (Q22-P22+1)/(Q22)*100</f>
+        <f xml:space="preserve"> (Q22-P22+1)/(Q22)*100</f>
         <v>98.319327731092429</v>
       </c>
-      <c r="S22" s="82" t="s">
+      <c r="S22" s="72" t="s">
         <v>39</v>
       </c>
       <c r="T22" s="3">
-        <f t="shared" si="1"/>
+        <f>N22-L22</f>
         <v>16.32</v>
       </c>
     </row>
@@ -6295,10 +6343,10 @@
       <c r="B23" s="3">
         <v>22</v>
       </c>
-      <c r="C23" s="67" t="s">
+      <c r="C23" s="80" t="s">
         <v>40</v>
       </c>
-      <c r="D23" s="68"/>
+      <c r="D23" s="81"/>
       <c r="E23" s="12">
         <v>58</v>
       </c>
@@ -6326,7 +6374,7 @@
       <c r="M23" s="17">
         <v>30.77</v>
       </c>
-      <c r="N23" s="85">
+      <c r="N23" s="75">
         <v>73.34</v>
       </c>
       <c r="O23" s="18">
@@ -6335,18 +6383,18 @@
       <c r="P23" s="19">
         <v>10</v>
       </c>
-      <c r="Q23" s="81">
+      <c r="Q23" s="71">
         <v>88</v>
       </c>
       <c r="R23" s="3">
-        <f t="shared" si="2"/>
+        <f xml:space="preserve"> (Q23-P23+1)/(Q23)*100</f>
         <v>89.772727272727266</v>
       </c>
-      <c r="S23" s="82" t="s">
+      <c r="S23" s="72" t="s">
         <v>39</v>
       </c>
       <c r="T23" s="3">
-        <f t="shared" si="1"/>
+        <f>N23-L23</f>
         <v>8.9900000000000091</v>
       </c>
     </row>
@@ -6357,10 +6405,10 @@
       <c r="B24" s="3">
         <v>23</v>
       </c>
-      <c r="C24" s="67" t="s">
+      <c r="C24" s="80" t="s">
         <v>41</v>
       </c>
-      <c r="D24" s="68"/>
+      <c r="D24" s="81"/>
       <c r="E24" s="12">
         <v>64</v>
       </c>
@@ -6388,7 +6436,7 @@
       <c r="M24" s="17">
         <v>26.27</v>
       </c>
-      <c r="N24" s="85">
+      <c r="N24" s="75">
         <v>77.680000000000007</v>
       </c>
       <c r="O24" s="18">
@@ -6397,30 +6445,32 @@
       <c r="P24" s="19">
         <v>6</v>
       </c>
-      <c r="Q24" s="81">
+      <c r="Q24" s="71">
         <v>52</v>
       </c>
       <c r="R24" s="3">
-        <f t="shared" si="2"/>
+        <f xml:space="preserve"> (Q24-P24+1)/(Q24)*100</f>
         <v>90.384615384615387</v>
       </c>
-      <c r="S24" s="82" t="s">
+      <c r="S24" s="72" t="s">
         <v>42</v>
       </c>
       <c r="T24" s="3">
-        <f t="shared" si="1"/>
+        <f>N24-L24</f>
         <v>9.6500000000000057</v>
       </c>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A25" s="31"/>
+      <c r="A25" s="31">
+        <v>44857</v>
+      </c>
       <c r="B25" s="3">
         <v>24</v>
       </c>
-      <c r="C25" s="67" t="s">
+      <c r="C25" s="80" t="s">
         <v>43</v>
       </c>
-      <c r="D25" s="68"/>
+      <c r="D25" s="81"/>
       <c r="E25" s="12">
         <v>63</v>
       </c>
@@ -6448,7 +6498,7 @@
       <c r="M25" s="17">
         <v>35.83</v>
       </c>
-      <c r="N25" s="85">
+      <c r="N25" s="75">
         <v>62.03</v>
       </c>
       <c r="O25" s="18">
@@ -6457,51 +6507,80 @@
       <c r="P25" s="19">
         <v>3</v>
       </c>
-      <c r="Q25" s="81">
+      <c r="Q25" s="71">
         <v>26</v>
       </c>
       <c r="R25" s="3">
-        <f t="shared" si="2"/>
+        <f xml:space="preserve"> (Q25-P25+1)/(Q25)*100</f>
         <v>92.307692307692307</v>
       </c>
-      <c r="S25" s="82" t="s">
+      <c r="S25" s="72" t="s">
         <v>42</v>
       </c>
       <c r="T25" s="3">
-        <f t="shared" si="1"/>
+        <f>N25-L25</f>
         <v>0.32999999999999829</v>
       </c>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A26" s="31"/>
-      <c r="B26" s="3">
+      <c r="A26" s="31">
+        <v>44871</v>
+      </c>
+      <c r="B26" s="90">
         <v>25</v>
       </c>
-      <c r="C26" s="67" t="s">
+      <c r="C26" s="80" t="s">
         <v>44</v>
       </c>
-      <c r="D26" s="68"/>
-      <c r="E26" s="12"/>
-      <c r="F26" s="13"/>
-      <c r="G26" s="14"/>
-      <c r="H26" s="32"/>
-      <c r="I26" s="19"/>
-      <c r="J26" s="28"/>
-      <c r="K26" s="33"/>
-      <c r="L26" s="16"/>
-      <c r="M26" s="17"/>
-      <c r="N26" s="85"/>
-      <c r="O26" s="18"/>
-      <c r="P26" s="19"/>
-      <c r="Q26" s="81"/>
-      <c r="R26" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S26" s="82"/>
+      <c r="D26" s="81"/>
+      <c r="E26" s="12">
+        <v>63</v>
+      </c>
+      <c r="F26" s="13">
+        <v>45</v>
+      </c>
+      <c r="G26" s="14">
+        <v>18</v>
+      </c>
+      <c r="H26" s="32">
+        <v>2</v>
+      </c>
+      <c r="I26" s="19">
+        <v>69</v>
+      </c>
+      <c r="J26" s="28">
+        <v>-2.64</v>
+      </c>
+      <c r="K26" s="33">
+        <v>3</v>
+      </c>
+      <c r="L26" s="16">
+        <v>66.36</v>
+      </c>
+      <c r="M26" s="17">
+        <v>47.2</v>
+      </c>
+      <c r="N26" s="75">
+        <v>75.02</v>
+      </c>
+      <c r="O26" s="18">
+        <v>71.430000000000007</v>
+      </c>
+      <c r="P26" s="19">
+        <v>7</v>
+      </c>
+      <c r="Q26" s="71">
+        <v>40</v>
+      </c>
+      <c r="R26" s="3">
+        <v>85</v>
+      </c>
+      <c r="S26" s="72" t="s">
+        <v>42</v>
+      </c>
       <c r="T26" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>N26-L26</f>
+        <v>8.6599999999999966</v>
       </c>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.3">
@@ -6509,10 +6588,10 @@
       <c r="B27" s="3">
         <v>26</v>
       </c>
-      <c r="C27" s="67" t="s">
+      <c r="C27" s="80" t="s">
         <v>45</v>
       </c>
-      <c r="D27" s="68"/>
+      <c r="D27" s="81"/>
       <c r="E27" s="12"/>
       <c r="F27" s="13"/>
       <c r="G27" s="14"/>
@@ -6522,17 +6601,17 @@
       <c r="K27" s="33"/>
       <c r="L27" s="16"/>
       <c r="M27" s="17"/>
-      <c r="N27" s="85"/>
+      <c r="N27" s="75"/>
       <c r="O27" s="18"/>
       <c r="P27" s="19"/>
-      <c r="Q27" s="81"/>
+      <c r="Q27" s="71"/>
       <c r="R27" s="3" t="e">
-        <f t="shared" si="2"/>
+        <f xml:space="preserve"> (Q27-P27+1)/(Q27)*100</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="S27" s="82"/>
+      <c r="S27" s="72"/>
       <c r="T27" s="3">
-        <f t="shared" si="1"/>
+        <f>N27-L27</f>
         <v>0</v>
       </c>
     </row>
@@ -6541,10 +6620,10 @@
       <c r="B28" s="3">
         <v>27</v>
       </c>
-      <c r="C28" s="67" t="s">
+      <c r="C28" s="80" t="s">
         <v>46</v>
       </c>
-      <c r="D28" s="68"/>
+      <c r="D28" s="81"/>
       <c r="E28" s="12"/>
       <c r="F28" s="13"/>
       <c r="G28" s="14"/>
@@ -6554,17 +6633,17 @@
       <c r="K28" s="33"/>
       <c r="L28" s="16"/>
       <c r="M28" s="17"/>
-      <c r="N28" s="85"/>
+      <c r="N28" s="75"/>
       <c r="O28" s="18"/>
       <c r="P28" s="19"/>
-      <c r="Q28" s="81"/>
+      <c r="Q28" s="71"/>
       <c r="R28" s="3" t="e">
-        <f t="shared" si="2"/>
+        <f xml:space="preserve"> (Q28-P28+1)/(Q28)*100</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="S28" s="82"/>
+      <c r="S28" s="72"/>
       <c r="T28" s="3">
-        <f t="shared" si="1"/>
+        <f>N28-L28</f>
         <v>0</v>
       </c>
     </row>
@@ -6573,10 +6652,10 @@
       <c r="B29" s="3">
         <v>28</v>
       </c>
-      <c r="C29" s="67" t="s">
+      <c r="C29" s="80" t="s">
         <v>47</v>
       </c>
-      <c r="D29" s="68"/>
+      <c r="D29" s="81"/>
       <c r="E29" s="12"/>
       <c r="F29" s="13"/>
       <c r="G29" s="14"/>
@@ -6586,17 +6665,17 @@
       <c r="K29" s="33"/>
       <c r="L29" s="16"/>
       <c r="M29" s="17"/>
-      <c r="N29" s="85"/>
+      <c r="N29" s="75"/>
       <c r="O29" s="18"/>
       <c r="P29" s="19"/>
-      <c r="Q29" s="81"/>
+      <c r="Q29" s="71"/>
       <c r="R29" s="3" t="e">
-        <f t="shared" si="2"/>
+        <f xml:space="preserve"> (Q29-P29+1)/(Q29)*100</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="S29" s="82"/>
+      <c r="S29" s="72"/>
       <c r="T29" s="3">
-        <f t="shared" si="1"/>
+        <f>N29-L29</f>
         <v>0</v>
       </c>
     </row>
@@ -6605,10 +6684,10 @@
       <c r="B30" s="3">
         <v>29</v>
       </c>
-      <c r="C30" s="67" t="s">
+      <c r="C30" s="80" t="s">
         <v>48</v>
       </c>
-      <c r="D30" s="68"/>
+      <c r="D30" s="81"/>
       <c r="E30" s="12"/>
       <c r="F30" s="13"/>
       <c r="G30" s="14"/>
@@ -6618,17 +6697,17 @@
       <c r="K30" s="33"/>
       <c r="L30" s="16"/>
       <c r="M30" s="17"/>
-      <c r="N30" s="85"/>
+      <c r="N30" s="75"/>
       <c r="O30" s="18"/>
       <c r="P30" s="19"/>
-      <c r="Q30" s="81"/>
+      <c r="Q30" s="71"/>
       <c r="R30" s="3" t="e">
-        <f t="shared" si="2"/>
+        <f xml:space="preserve"> (Q30-P30+1)/(Q30)*100</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="S30" s="82"/>
+      <c r="S30" s="72"/>
       <c r="T30" s="3">
-        <f t="shared" si="1"/>
+        <f>N30-L30</f>
         <v>0</v>
       </c>
     </row>
@@ -6637,10 +6716,10 @@
       <c r="B31" s="3">
         <v>30</v>
       </c>
-      <c r="C31" s="74" t="s">
+      <c r="C31" s="82" t="s">
         <v>49</v>
       </c>
-      <c r="D31" s="74"/>
+      <c r="D31" s="82"/>
       <c r="E31" s="12"/>
       <c r="F31" s="13"/>
       <c r="G31" s="14"/>
@@ -6650,16 +6729,16 @@
       <c r="K31" s="33"/>
       <c r="L31" s="16"/>
       <c r="M31" s="17"/>
-      <c r="N31" s="85"/>
+      <c r="N31" s="75"/>
       <c r="O31" s="18"/>
       <c r="P31" s="19"/>
-      <c r="Q31" s="81"/>
+      <c r="Q31" s="71"/>
       <c r="R31" s="3" t="e">
         <f xml:space="preserve"> (P31-O31+1)/(P31)*100</f>
         <v>#DIV/0!</v>
       </c>
       <c r="T31" s="3">
-        <f t="shared" si="1"/>
+        <f>N31-L31</f>
         <v>0</v>
       </c>
     </row>
@@ -6668,10 +6747,10 @@
       <c r="B32" s="3">
         <v>31</v>
       </c>
-      <c r="C32" s="74" t="s">
+      <c r="C32" s="82" t="s">
         <v>50</v>
       </c>
-      <c r="D32" s="74"/>
+      <c r="D32" s="82"/>
       <c r="E32" s="12"/>
       <c r="F32" s="13"/>
       <c r="G32" s="14"/>
@@ -6681,16 +6760,16 @@
       <c r="K32" s="33"/>
       <c r="L32" s="16"/>
       <c r="M32" s="17"/>
-      <c r="N32" s="85"/>
+      <c r="N32" s="75"/>
       <c r="O32" s="18"/>
       <c r="P32" s="19"/>
-      <c r="Q32" s="81"/>
+      <c r="Q32" s="71"/>
       <c r="R32" s="3" t="e">
         <f xml:space="preserve"> (P32-O32+1)/(P32)*100</f>
         <v>#DIV/0!</v>
       </c>
       <c r="T32" s="3">
-        <f t="shared" si="1"/>
+        <f>N32-L32</f>
         <v>0</v>
       </c>
     </row>
@@ -6699,10 +6778,10 @@
       <c r="B33" s="3">
         <v>32</v>
       </c>
-      <c r="C33" s="74" t="s">
+      <c r="C33" s="82" t="s">
         <v>51</v>
       </c>
-      <c r="D33" s="74"/>
+      <c r="D33" s="82"/>
       <c r="E33" s="12"/>
       <c r="F33" s="13"/>
       <c r="G33" s="14"/>
@@ -6712,16 +6791,16 @@
       <c r="K33" s="33"/>
       <c r="L33" s="16"/>
       <c r="M33" s="17"/>
-      <c r="N33" s="85"/>
+      <c r="N33" s="75"/>
       <c r="O33" s="18"/>
       <c r="P33" s="19"/>
-      <c r="Q33" s="81"/>
+      <c r="Q33" s="71"/>
       <c r="R33" s="3" t="e">
         <f xml:space="preserve"> (P33-O33+1)/(P33)*100</f>
         <v>#DIV/0!</v>
       </c>
       <c r="T33" s="3">
-        <f t="shared" si="1"/>
+        <f>N33-L33</f>
         <v>0</v>
       </c>
     </row>
@@ -6730,10 +6809,10 @@
       <c r="B34" s="3">
         <v>33</v>
       </c>
-      <c r="C34" s="74" t="s">
+      <c r="C34" s="82" t="s">
         <v>52</v>
       </c>
-      <c r="D34" s="74"/>
+      <c r="D34" s="82"/>
       <c r="E34" s="12"/>
       <c r="F34" s="13"/>
       <c r="G34" s="14"/>
@@ -6743,16 +6822,16 @@
       <c r="K34" s="33"/>
       <c r="L34" s="16"/>
       <c r="M34" s="17"/>
-      <c r="N34" s="85"/>
+      <c r="N34" s="75"/>
       <c r="O34" s="18"/>
       <c r="P34" s="19"/>
-      <c r="Q34" s="81"/>
+      <c r="Q34" s="71"/>
       <c r="R34" s="3" t="e">
         <f xml:space="preserve"> (P34-O34+1)/(P34)*100</f>
         <v>#DIV/0!</v>
       </c>
       <c r="T34" s="3">
-        <f t="shared" si="1"/>
+        <f>N34-L34</f>
         <v>0</v>
       </c>
     </row>
@@ -6761,62 +6840,62 @@
       <c r="B35" s="3">
         <v>34</v>
       </c>
-      <c r="C35" s="70" t="s">
+      <c r="C35" s="83" t="s">
         <v>21</v>
       </c>
-      <c r="D35" s="70"/>
+      <c r="D35" s="83"/>
       <c r="E35" s="12">
-        <f t="shared" ref="E35:O35" si="3">AVERAGE(E2:E34)</f>
-        <v>54.5</v>
+        <f t="shared" ref="E35:O35" si="1">AVERAGE(E2:E34)</f>
+        <v>54.84</v>
       </c>
       <c r="F35" s="13">
-        <f t="shared" si="3"/>
-        <v>40.695652173913047</v>
+        <f t="shared" si="1"/>
+        <v>40.875</v>
       </c>
       <c r="G35" s="14">
-        <f t="shared" si="3"/>
-        <v>14</v>
+        <f t="shared" si="1"/>
+        <v>14.16</v>
       </c>
       <c r="H35" s="15">
-        <f t="shared" si="3"/>
-        <v>10.5</v>
+        <f t="shared" si="1"/>
+        <v>10.16</v>
       </c>
       <c r="I35" s="19">
-        <f t="shared" si="3"/>
-        <v>60.458333333333336</v>
+        <f t="shared" si="1"/>
+        <v>60.8</v>
       </c>
       <c r="J35" s="28">
-        <f t="shared" si="3"/>
-        <v>-3.0566666666666666</v>
+        <f t="shared" si="1"/>
+        <v>-3.04</v>
       </c>
       <c r="K35" s="15">
-        <f t="shared" si="3"/>
-        <v>17.55</v>
+        <f t="shared" si="1"/>
+        <v>16.857142857142858</v>
       </c>
       <c r="L35" s="16">
-        <f t="shared" si="3"/>
-        <v>57.484583333333326</v>
+        <f t="shared" si="1"/>
+        <v>57.83959999999999</v>
       </c>
       <c r="M35" s="17">
-        <f t="shared" si="3"/>
-        <v>40.377391304347832</v>
-      </c>
-      <c r="N35" s="85">
-        <f t="shared" si="3"/>
-        <v>82.805833333333325</v>
+        <f t="shared" si="1"/>
+        <v>40.661666666666676</v>
+      </c>
+      <c r="N35" s="75">
+        <f t="shared" si="1"/>
+        <v>82.494399999999985</v>
       </c>
       <c r="O35" s="18">
-        <f t="shared" si="3"/>
-        <v>72.873500000000007</v>
+        <f t="shared" si="1"/>
+        <v>72.804761904761904</v>
       </c>
       <c r="P35" s="19">
         <f>AVERAGE(P2:P34)</f>
-        <v>140.56521739130434</v>
-      </c>
-      <c r="Q35" s="81"/>
+        <v>135</v>
+      </c>
+      <c r="Q35" s="71"/>
       <c r="T35" s="3">
-        <f t="shared" si="1"/>
-        <v>25.321249999999999</v>
+        <f>N35-L35</f>
+        <v>24.654799999999994</v>
       </c>
     </row>
     <row r="36" spans="1:20" x14ac:dyDescent="0.3">
@@ -6830,7 +6909,7 @@
       <c r="K36" s="23"/>
       <c r="L36" s="24"/>
       <c r="M36" s="25"/>
-      <c r="N36" s="88"/>
+      <c r="N36" s="78"/>
       <c r="O36" s="26"/>
       <c r="P36" s="27"/>
       <c r="Q36" s="27"/>
@@ -6846,7 +6925,7 @@
       <c r="K37" s="23"/>
       <c r="L37" s="24"/>
       <c r="M37" s="25"/>
-      <c r="N37" s="88"/>
+      <c r="N37" s="78"/>
       <c r="O37" s="26"/>
       <c r="P37" s="27"/>
       <c r="Q37" s="27"/>
@@ -6861,7 +6940,7 @@
       <c r="K38" s="23"/>
       <c r="L38" s="24"/>
       <c r="M38" s="25"/>
-      <c r="N38" s="88"/>
+      <c r="N38" s="78"/>
       <c r="O38" s="26"/>
       <c r="P38" s="27"/>
       <c r="Q38" s="27"/>
@@ -6876,7 +6955,7 @@
       <c r="K39" s="23"/>
       <c r="L39" s="24"/>
       <c r="M39" s="25"/>
-      <c r="N39" s="88"/>
+      <c r="N39" s="78"/>
       <c r="O39" s="26"/>
       <c r="P39" s="27"/>
       <c r="Q39" s="27"/>
@@ -6891,7 +6970,7 @@
       <c r="K40" s="23"/>
       <c r="L40" s="24"/>
       <c r="M40" s="25"/>
-      <c r="N40" s="88"/>
+      <c r="N40" s="78"/>
       <c r="O40" s="26"/>
       <c r="P40" s="27"/>
       <c r="Q40" s="27"/>
@@ -6906,23 +6985,22 @@
       <c r="K41" s="23"/>
       <c r="L41" s="24"/>
       <c r="M41" s="25"/>
-      <c r="N41" s="88"/>
+      <c r="N41" s="78"/>
       <c r="O41" s="26"/>
       <c r="P41" s="27"/>
       <c r="Q41" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C15:D15"/>
     <mergeCell ref="C35:D35"/>
     <mergeCell ref="C11:D11"/>
     <mergeCell ref="C1:D1"/>
@@ -6939,15 +7017,16 @@
     <mergeCell ref="C20:D20"/>
     <mergeCell ref="C21:D21"/>
     <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C34:D34"/>
   </mergeCells>
   <conditionalFormatting sqref="M2:M14">
     <cfRule type="colorScale" priority="52">
@@ -7028,23 +7107,23 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="54" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="7" priority="54" operator="greaterThan">
       <formula>$G$24</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P22:P24 P26:P30">
-    <cfRule type="cellIs" dxfId="14" priority="33" operator="between">
+    <cfRule type="cellIs" dxfId="6" priority="33" operator="between">
       <formula>1</formula>
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S22:S30">
-    <cfRule type="cellIs" dxfId="13" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="32" operator="equal">
       <formula>"NO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S22:S30">
-    <cfRule type="cellIs" dxfId="12" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="31" operator="equal">
       <formula>"YES"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7103,7 +7182,7 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="28" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="28" operator="greaterThan">
       <formula>$G$24</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7174,7 +7253,7 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="64" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="2" priority="64" operator="greaterThan">
       <formula>$F$35</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7238,7 +7317,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J25">
-    <cfRule type="iconSet" priority="11">
+    <cfRule type="iconSet" priority="67">
       <iconSet iconSet="3Arrows">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="33"/>
@@ -7247,7 +7326,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F25">
-    <cfRule type="colorScale" priority="12">
+    <cfRule type="colorScale" priority="68">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -7257,12 +7336,12 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="13" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="68" operator="greaterThan">
       <formula>$G$24</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P25">
-    <cfRule type="cellIs" dxfId="8" priority="6" operator="between">
+    <cfRule type="cellIs" dxfId="0" priority="6" operator="between">
       <formula>1</formula>
       <formula>10</formula>
     </cfRule>

</xml_diff>

<commit_message>
Gave GO classes mock 5.
</commit_message>
<xml_diff>
--- a/My Marks Tracker.xlsx
+++ b/My Marks Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GATE 2022 &amp; 2023\My Progress trackers &amp; Journey - In Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48D4814E-53B1-4D27-B2D6-DFD8B141F354}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC9616B7-C1A0-4713-9CDC-27451F565A70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3209D17C-0F5C-4895-BA2D-FBE4C1879A87}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="59">
   <si>
     <t>Test Name</t>
   </si>
@@ -64,9 +64,6 @@
   </si>
   <si>
     <t>Test No.</t>
-  </si>
-  <si>
-    <t>Unatt Marks</t>
   </si>
   <si>
     <t>Topper</t>
@@ -197,12 +194,21 @@
   <si>
     <t>GO CLASSES MOCK - 4</t>
   </si>
+  <si>
+    <t>GO CLASSES MOCK - 5</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>Analyzed?</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -225,8 +231,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="16">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -284,18 +296,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -540,9 +540,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -557,15 +557,6 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -613,12 +604,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -648,26 +633,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -679,32 +648,32 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="13" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="11" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="13" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="11" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="13" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="11" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -716,52 +685,88 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -769,7 +774,7 @@
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="16">
+  <dxfs count="24">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -777,6 +782,57 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="-0.24994659260841701"/>
         </patternFill>
       </fill>
     </dxf>
@@ -825,9 +881,29 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
       <fill>
         <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="-0.24994659260841701"/>
         </patternFill>
       </fill>
     </dxf>
@@ -986,7 +1062,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$L$1</c:f>
+              <c:f>Sheet1!$K$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1109,7 +1185,7 @@
           </c:trendline>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$L$2:$L$38</c:f>
+              <c:f>Sheet1!$K$2:$K$38</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="37"/>
@@ -1194,6 +1270,9 @@
                 <c:pt idx="26">
                   <c:v>83.35</c:v>
                 </c:pt>
+                <c:pt idx="28">
+                  <c:v>74.69</c:v>
+                </c:pt>
                 <c:pt idx="29">
                   <c:v>59.33</c:v>
                 </c:pt>
@@ -1202,6 +1281,9 @@
                 </c:pt>
                 <c:pt idx="31">
                   <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>70.66</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1540,7 +1622,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$O$1</c:f>
+              <c:f>Sheet1!$N$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1561,7 +1643,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$O$2:$O$38</c:f>
+              <c:f>Sheet1!$N$2:$N$38</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="37"/>
@@ -1633,6 +1715,9 @@
                 </c:pt>
                 <c:pt idx="26">
                   <c:v>86.15</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>80.95</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1849,14 +1934,14 @@
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
-        <c:grouping val="standard"/>
+        <c:grouping val="stacked"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$T$1</c:f>
+              <c:f>Sheet1!$S$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1875,11 +1960,23 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$T$2:$T$38</c:f>
+              <c:f>Sheet1!$S$2:$S$38</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="37"/>
@@ -1968,7 +2065,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0</c:v>
+                  <c:v>11.310000000000002</c:v>
                 </c:pt>
                 <c:pt idx="29">
                   <c:v>21.67</c:v>
@@ -1980,7 +2077,7 @@
                   <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0</c:v>
+                  <c:v>0.67000000000000171</c:v>
                 </c:pt>
                 <c:pt idx="33">
                   <c:v>0</c:v>
@@ -2012,6 +2109,7 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
         <c:axId val="278380368"/>
         <c:axId val="278375792"/>
@@ -2221,7 +2319,7 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:areaChart>
+      <c:lineChart>
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
@@ -2229,7 +2327,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$R$1</c:f>
+              <c:f>Sheet1!$Q$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2239,34 +2337,11 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:gradFill rotWithShape="1">
-              <a:gsLst>
-                <a:gs pos="0">
-                  <a:schemeClr val="accent1">
-                    <a:satMod val="103000"/>
-                    <a:lumMod val="102000"/>
-                    <a:tint val="94000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="50000">
-                  <a:schemeClr val="accent1">
-                    <a:satMod val="110000"/>
-                    <a:lumMod val="100000"/>
-                    <a:shade val="100000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="100000">
-                  <a:schemeClr val="accent1">
-                    <a:lumMod val="99000"/>
-                    <a:satMod val="120000"/>
-                    <a:shade val="78000"/>
-                  </a:schemeClr>
-                </a:gs>
-              </a:gsLst>
-              <a:lin ang="5400000" scaled="0"/>
-            </a:gradFill>
-            <a:ln>
-              <a:noFill/>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
             </a:ln>
             <a:effectLst>
               <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
@@ -2276,9 +2351,12 @@
               </a:outerShdw>
             </a:effectLst>
           </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$R$2:$R$45</c:f>
+              <c:f>Sheet1!$Q$2:$Q$45</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="44"/>
@@ -2367,7 +2445,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0</c:v>
+                  <c:v>95.081967213114751</c:v>
                 </c:pt>
                 <c:pt idx="29">
                   <c:v>74.336283185840713</c:v>
@@ -2379,7 +2457,7 @@
                   <c:v>92.64705882352942</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0</c:v>
+                  <c:v>97.674418604651152</c:v>
                 </c:pt>
                 <c:pt idx="33">
                   <c:v>0</c:v>
@@ -2399,6 +2477,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-964A-42BC-B88F-B2E79615D280}"/>
@@ -2413,9 +2492,10 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:smooth val="0"/>
         <c:axId val="930156304"/>
         <c:axId val="930143824"/>
-      </c:areaChart>
+      </c:lineChart>
       <c:catAx>
         <c:axId val="930156304"/>
         <c:scaling>
@@ -2518,7 +2598,7 @@
         </c:txPr>
         <c:crossAx val="930156304"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
+        <c:crossBetween val="between"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -4785,7 +4865,7 @@
       <xdr:rowOff>144556</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>12</xdr:col>
       <xdr:colOff>542813</xdr:colOff>
       <xdr:row>59</xdr:row>
       <xdr:rowOff>144556</xdr:rowOff>
@@ -4815,13 +4895,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>22412</xdr:colOff>
       <xdr:row>45</xdr:row>
       <xdr:rowOff>170330</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
+      <xdr:col>19</xdr:col>
       <xdr:colOff>354106</xdr:colOff>
       <xdr:row>61</xdr:row>
       <xdr:rowOff>44824</xdr:rowOff>
@@ -4851,16 +4931,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>103093</xdr:colOff>
-      <xdr:row>64</xdr:row>
-      <xdr:rowOff>161365</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>551328</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>170330</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>67235</xdr:colOff>
-      <xdr:row>80</xdr:row>
-      <xdr:rowOff>35860</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>44822</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>107577</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5185,10 +5265,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E08F6CAB-EED7-4179-B275-45A8F5F85EF1}">
-  <dimension ref="A1:T45"/>
+  <dimension ref="A1:S45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L30" sqref="L30"/>
+    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="R72" sqref="R72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5202,2180 +5282,2286 @@
     <col min="7" max="7" width="9.77734375" style="8" customWidth="1"/>
     <col min="8" max="8" width="8.44140625" style="5" customWidth="1"/>
     <col min="9" max="9" width="10.44140625" style="7" customWidth="1"/>
-    <col min="10" max="10" width="8.88671875" style="30"/>
-    <col min="11" max="11" width="12.6640625" style="5" customWidth="1"/>
-    <col min="12" max="12" width="8.88671875" style="6"/>
-    <col min="13" max="13" width="17.77734375" style="9" customWidth="1"/>
-    <col min="14" max="14" width="8.88671875" style="79"/>
-    <col min="15" max="15" width="10.5546875" style="10" customWidth="1"/>
-    <col min="16" max="17" width="8.88671875" style="7"/>
-    <col min="18" max="18" width="11.77734375" style="3" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.88671875" style="27"/>
+    <col min="11" max="11" width="8.88671875" style="6"/>
+    <col min="12" max="12" width="17.77734375" style="9" customWidth="1"/>
+    <col min="13" max="13" width="8.88671875" style="68"/>
+    <col min="14" max="14" width="10.5546875" style="10" customWidth="1"/>
+    <col min="15" max="16" width="8.88671875" style="7"/>
+    <col min="17" max="17" width="11.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="11" customFormat="1" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="34" t="s">
+    <row r="1" spans="1:19" s="11" customFormat="1" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="86" t="s">
+      <c r="C1" s="72" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="86"/>
-      <c r="E1" s="35" t="s">
+      <c r="D1" s="72"/>
+      <c r="E1" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="36" t="s">
+      <c r="F1" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="37" t="s">
+      <c r="G1" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="38" t="s">
+      <c r="H1" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="39" t="s">
+      <c r="I1" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="40" t="s">
+      <c r="J1" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="38" t="s">
+      <c r="K1" s="36" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="M1" s="62" t="s">
         <v>13</v>
       </c>
-      <c r="L1" s="41" t="s">
-        <v>6</v>
-      </c>
-      <c r="M1" s="42" t="s">
-        <v>23</v>
-      </c>
-      <c r="N1" s="73" t="s">
+      <c r="N1" s="38" t="s">
+        <v>7</v>
+      </c>
+      <c r="O1" s="34" t="s">
+        <v>2</v>
+      </c>
+      <c r="P1" s="55" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q1" s="69" t="s">
+        <v>52</v>
+      </c>
+      <c r="R1" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="S1" s="54" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="45"/>
+      <c r="B2" s="46">
+        <v>1</v>
+      </c>
+      <c r="C2" s="73" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="73"/>
+      <c r="E2" s="76">
+        <v>41</v>
+      </c>
+      <c r="F2" s="76">
+        <v>27</v>
+      </c>
+      <c r="G2" s="77">
+        <f>E2-F2</f>
         <v>14</v>
       </c>
-      <c r="O1" s="43" t="s">
-        <v>7</v>
-      </c>
-      <c r="P1" s="39" t="s">
+      <c r="H2" s="47">
+        <f>65-E2</f>
+        <v>24</v>
+      </c>
+      <c r="I2" s="47">
+        <v>40</v>
+      </c>
+      <c r="J2" s="47">
+        <v>-4.29</v>
+      </c>
+      <c r="K2" s="47">
+        <v>35.71</v>
+      </c>
+      <c r="L2" s="47">
+        <v>39.869999999999997</v>
+      </c>
+      <c r="M2" s="63">
+        <v>86.34</v>
+      </c>
+      <c r="N2" s="47">
+        <v>65.849999999999994</v>
+      </c>
+      <c r="O2" s="47">
+        <v>157</v>
+      </c>
+      <c r="P2" s="56">
+        <v>268</v>
+      </c>
+      <c r="Q2" s="3">
+        <f t="shared" ref="Q2:Q21" si="0" xml:space="preserve"> (P2-O2+1)/(P2)*100</f>
+        <v>41.791044776119399</v>
+      </c>
+      <c r="R2" s="61" t="s">
+        <v>38</v>
+      </c>
+      <c r="S2" s="3">
+        <f t="shared" ref="S2:S39" si="1">M2-K2</f>
+        <v>50.63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="48"/>
+      <c r="B3" s="49">
         <v>2</v>
       </c>
-      <c r="Q1" s="66" t="s">
-        <v>22</v>
-      </c>
-      <c r="R1" s="80" t="s">
-        <v>53</v>
-      </c>
-      <c r="T1" s="65" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="56"/>
-      <c r="B2" s="57">
-        <v>1</v>
-      </c>
-      <c r="C2" s="87" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="87"/>
-      <c r="E2" s="58">
+      <c r="C3" s="70" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="70"/>
+      <c r="E3" s="77">
+        <v>40</v>
+      </c>
+      <c r="F3" s="77">
+        <v>27</v>
+      </c>
+      <c r="G3" s="77">
+        <f t="shared" ref="G3:G10" si="2">E3-F3</f>
+        <v>13</v>
+      </c>
+      <c r="H3" s="47">
+        <f>65-E3</f>
+        <v>25</v>
+      </c>
+      <c r="I3" s="50">
         <v>41</v>
       </c>
-      <c r="F2" s="58">
-        <v>27</v>
-      </c>
-      <c r="G2" s="58">
-        <v>14</v>
-      </c>
-      <c r="H2" s="58">
-        <v>24</v>
-      </c>
-      <c r="I2" s="58">
-        <v>40</v>
-      </c>
-      <c r="J2" s="58">
-        <v>-4.29</v>
-      </c>
-      <c r="K2" s="58">
-        <v>39</v>
-      </c>
-      <c r="L2" s="58">
-        <v>35.71</v>
-      </c>
-      <c r="M2" s="58">
-        <v>39.869999999999997</v>
-      </c>
-      <c r="N2" s="74">
-        <v>86.34</v>
-      </c>
-      <c r="O2" s="58">
-        <v>65.849999999999994</v>
-      </c>
-      <c r="P2" s="58">
-        <v>157</v>
-      </c>
-      <c r="Q2" s="67">
-        <v>268</v>
-      </c>
-      <c r="R2" s="3">
-        <f t="shared" ref="R2:R21" si="0" xml:space="preserve"> (Q2-P2+1)/(Q2)*100</f>
-        <v>41.791044776119399</v>
-      </c>
-      <c r="T2" s="3">
-        <f t="shared" ref="T2:T39" si="1">N2-L2</f>
-        <v>50.63</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A3" s="59"/>
-      <c r="B3" s="60">
-        <v>2</v>
-      </c>
-      <c r="C3" s="85" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="85"/>
-      <c r="E3" s="61">
-        <v>40</v>
-      </c>
-      <c r="F3" s="61">
-        <v>27</v>
-      </c>
-      <c r="G3" s="61">
-        <v>13</v>
-      </c>
-      <c r="H3" s="61">
-        <v>25</v>
-      </c>
-      <c r="I3" s="61">
-        <v>41</v>
-      </c>
-      <c r="J3" s="61">
+      <c r="J3" s="50">
         <v>-3.3</v>
       </c>
-      <c r="K3" s="61">
-        <v>41</v>
-      </c>
-      <c r="L3" s="61">
+      <c r="K3" s="50">
         <v>37.700000000000003</v>
       </c>
-      <c r="M3" s="61">
+      <c r="L3" s="50">
         <v>39.18</v>
       </c>
-      <c r="N3" s="75">
+      <c r="M3" s="64">
         <v>84.69</v>
       </c>
-      <c r="O3" s="61">
+      <c r="N3" s="50">
         <v>67.5</v>
       </c>
-      <c r="P3" s="61">
+      <c r="O3" s="50">
         <v>114</v>
       </c>
-      <c r="Q3" s="68">
+      <c r="P3" s="57">
         <v>201</v>
       </c>
-      <c r="R3" s="3">
+      <c r="Q3" s="3">
         <f t="shared" si="0"/>
         <v>43.781094527363187</v>
       </c>
-      <c r="T3" s="3">
+      <c r="R3" s="61" t="s">
+        <v>38</v>
+      </c>
+      <c r="S3" s="3">
         <f t="shared" si="1"/>
         <v>46.989999999999995</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A4" s="59"/>
-      <c r="B4" s="60">
+    <row r="4" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="48"/>
+      <c r="B4" s="49">
         <v>3</v>
       </c>
-      <c r="C4" s="85" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="85"/>
-      <c r="E4" s="61">
+      <c r="C4" s="70" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="70"/>
+      <c r="E4" s="77">
         <v>51</v>
       </c>
-      <c r="F4" s="61">
+      <c r="F4" s="77">
         <v>33</v>
       </c>
-      <c r="G4" s="61">
+      <c r="G4" s="77">
+        <f>E4-F4</f>
         <v>18</v>
       </c>
-      <c r="H4" s="61">
+      <c r="H4" s="47">
+        <f t="shared" ref="H4:H34" si="3">65-E4</f>
         <v>14</v>
       </c>
-      <c r="I4" s="61">
+      <c r="I4" s="50">
         <v>52</v>
       </c>
-      <c r="J4" s="61">
+      <c r="J4" s="50">
         <v>-4.62</v>
       </c>
-      <c r="K4" s="61">
-        <v>24</v>
-      </c>
-      <c r="L4" s="61">
+      <c r="K4" s="50">
         <v>47.38</v>
       </c>
-      <c r="M4" s="61">
+      <c r="L4" s="50">
         <v>33.14</v>
       </c>
-      <c r="N4" s="75">
+      <c r="M4" s="64">
         <v>81.7</v>
       </c>
-      <c r="O4" s="61">
+      <c r="N4" s="50">
         <v>64.709999999999994</v>
       </c>
-      <c r="P4" s="61">
+      <c r="O4" s="50">
         <v>285</v>
       </c>
-      <c r="Q4" s="68">
+      <c r="P4" s="57">
         <v>1233</v>
       </c>
-      <c r="R4" s="3">
+      <c r="Q4" s="3">
         <f t="shared" si="0"/>
         <v>76.966747769667478</v>
       </c>
-      <c r="T4" s="3">
+      <c r="R4" s="61" t="s">
+        <v>38</v>
+      </c>
+      <c r="S4" s="3">
         <f t="shared" si="1"/>
         <v>34.32</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A5" s="59"/>
-      <c r="B5" s="60">
+    <row r="5" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="48"/>
+      <c r="B5" s="49">
         <v>4</v>
       </c>
-      <c r="C5" s="85" t="s">
+      <c r="C5" s="70" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="70"/>
+      <c r="E5" s="77">
+        <v>51</v>
+      </c>
+      <c r="F5" s="77" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="85"/>
-      <c r="E5" s="61">
-        <v>51</v>
-      </c>
-      <c r="F5" s="61" t="s">
-        <v>18</v>
-      </c>
-      <c r="G5" s="61">
+      <c r="G5" s="77">
         <v>15</v>
       </c>
-      <c r="H5" s="61">
+      <c r="H5" s="47">
+        <f t="shared" si="3"/>
         <v>14</v>
       </c>
-      <c r="I5" s="61">
+      <c r="I5" s="50">
         <v>54</v>
       </c>
-      <c r="J5" s="61">
+      <c r="J5" s="50">
         <v>-3.67</v>
       </c>
-      <c r="K5" s="61"/>
-      <c r="L5" s="61">
+      <c r="K5" s="50">
         <v>52.33</v>
       </c>
-      <c r="M5" s="61"/>
-      <c r="N5" s="75">
+      <c r="L5" s="50"/>
+      <c r="M5" s="64">
         <v>91</v>
       </c>
-      <c r="O5" s="61"/>
-      <c r="P5" s="61"/>
-      <c r="Q5" s="68"/>
-      <c r="R5" s="3" t="e">
+      <c r="N5" s="50"/>
+      <c r="O5" s="50"/>
+      <c r="P5" s="57"/>
+      <c r="Q5" s="3" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="T5" s="3">
+      <c r="R5" s="61" t="s">
+        <v>38</v>
+      </c>
+      <c r="S5" s="3">
         <f t="shared" si="1"/>
         <v>38.67</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A6" s="59"/>
-      <c r="B6" s="60">
+    <row r="6" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="48"/>
+      <c r="B6" s="49">
         <v>5</v>
       </c>
-      <c r="C6" s="85" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="85"/>
-      <c r="E6" s="61">
+      <c r="C6" s="70" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="70"/>
+      <c r="E6" s="77">
         <v>47</v>
       </c>
-      <c r="F6" s="61">
+      <c r="F6" s="77">
         <v>35</v>
       </c>
-      <c r="G6" s="61">
+      <c r="G6" s="77">
+        <f t="shared" si="2"/>
         <v>12</v>
       </c>
-      <c r="H6" s="61">
+      <c r="H6" s="47">
+        <f t="shared" si="3"/>
         <v>18</v>
       </c>
-      <c r="I6" s="61">
+      <c r="I6" s="50">
         <v>51</v>
       </c>
-      <c r="J6" s="61">
+      <c r="J6" s="50">
         <v>-1.65</v>
       </c>
-      <c r="K6" s="61">
-        <v>33</v>
-      </c>
-      <c r="L6" s="61">
+      <c r="K6" s="50">
         <v>49.35</v>
       </c>
-      <c r="M6" s="61">
+      <c r="L6" s="50">
         <v>39.799999999999997</v>
       </c>
-      <c r="N6" s="75">
+      <c r="M6" s="64">
         <v>87.36</v>
       </c>
-      <c r="O6" s="61">
+      <c r="N6" s="50">
         <v>74.47</v>
       </c>
-      <c r="P6" s="61">
+      <c r="O6" s="50">
         <v>290</v>
       </c>
-      <c r="Q6" s="68">
+      <c r="P6" s="57">
         <v>913</v>
       </c>
-      <c r="R6" s="3">
+      <c r="Q6" s="3">
         <f t="shared" si="0"/>
         <v>68.346111719605702</v>
       </c>
-      <c r="T6" s="3">
+      <c r="R6" s="61" t="s">
+        <v>38</v>
+      </c>
+      <c r="S6" s="3">
         <f t="shared" si="1"/>
         <v>38.01</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A7" s="59"/>
-      <c r="B7" s="60">
+    <row r="7" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="48"/>
+      <c r="B7" s="49">
         <v>6</v>
       </c>
-      <c r="C7" s="85" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" s="85"/>
-      <c r="E7" s="61">
+      <c r="C7" s="70" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="70"/>
+      <c r="E7" s="77">
         <v>51</v>
       </c>
-      <c r="F7" s="61">
+      <c r="F7" s="77">
         <v>35</v>
       </c>
-      <c r="G7" s="61">
+      <c r="G7" s="77">
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
-      <c r="H7" s="61">
+      <c r="H7" s="47">
+        <f t="shared" si="3"/>
         <v>14</v>
       </c>
-      <c r="I7" s="61">
+      <c r="I7" s="50">
         <v>51</v>
       </c>
-      <c r="J7" s="61">
+      <c r="J7" s="50">
         <v>-3.3</v>
       </c>
-      <c r="K7" s="61">
-        <v>24</v>
-      </c>
-      <c r="L7" s="61">
+      <c r="K7" s="50">
         <v>47.7</v>
       </c>
-      <c r="M7" s="61">
+      <c r="L7" s="50">
         <v>37.15</v>
       </c>
-      <c r="N7" s="75">
+      <c r="M7" s="64">
         <v>79.67</v>
       </c>
-      <c r="O7" s="61">
+      <c r="N7" s="50">
         <v>68.63</v>
       </c>
-      <c r="P7" s="61">
+      <c r="O7" s="50">
         <v>186</v>
       </c>
-      <c r="Q7" s="68">
+      <c r="P7" s="57">
         <v>714</v>
       </c>
-      <c r="R7" s="3">
+      <c r="Q7" s="3">
         <f t="shared" si="0"/>
         <v>74.089635854341736</v>
       </c>
-      <c r="T7" s="3">
+      <c r="R7" s="61" t="s">
+        <v>38</v>
+      </c>
+      <c r="S7" s="3">
         <f t="shared" si="1"/>
         <v>31.97</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A8" s="59"/>
-      <c r="B8" s="60">
+    <row r="8" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="48"/>
+      <c r="B8" s="49">
         <v>7</v>
       </c>
-      <c r="C8" s="85" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="85"/>
-      <c r="E8" s="61">
+      <c r="C8" s="70" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="70"/>
+      <c r="E8" s="77">
         <v>52</v>
       </c>
-      <c r="F8" s="61">
+      <c r="F8" s="77">
         <v>38</v>
       </c>
-      <c r="G8" s="61">
+      <c r="G8" s="77">
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
-      <c r="H8" s="61">
+      <c r="H8" s="47">
+        <f t="shared" si="3"/>
         <v>13</v>
       </c>
-      <c r="I8" s="61">
+      <c r="I8" s="50">
         <v>56</v>
       </c>
-      <c r="J8" s="61">
+      <c r="J8" s="50">
         <v>-4.29</v>
       </c>
-      <c r="K8" s="61">
-        <v>23</v>
-      </c>
-      <c r="L8" s="61">
+      <c r="K8" s="50">
         <v>51.71</v>
       </c>
-      <c r="M8" s="61">
+      <c r="L8" s="50">
         <v>44.06</v>
       </c>
-      <c r="N8" s="75">
+      <c r="M8" s="64">
         <v>88.02</v>
       </c>
-      <c r="O8" s="61">
+      <c r="N8" s="50">
         <v>73.08</v>
       </c>
-      <c r="P8" s="61">
+      <c r="O8" s="50">
         <v>207</v>
       </c>
-      <c r="Q8" s="68">
+      <c r="P8" s="57">
         <v>549</v>
       </c>
-      <c r="R8" s="3">
+      <c r="Q8" s="3">
         <f t="shared" si="0"/>
         <v>62.477231329690341</v>
       </c>
-      <c r="T8" s="3">
+      <c r="R8" s="61" t="s">
+        <v>38</v>
+      </c>
+      <c r="S8" s="3">
         <f t="shared" si="1"/>
         <v>36.309999999999995</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A9" s="59"/>
-      <c r="B9" s="60">
+    <row r="9" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="48"/>
+      <c r="B9" s="49">
         <v>8</v>
       </c>
-      <c r="C9" s="85" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" s="85"/>
-      <c r="E9" s="61">
+      <c r="C9" s="70" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="70"/>
+      <c r="E9" s="77">
         <v>55</v>
       </c>
-      <c r="F9" s="61">
+      <c r="F9" s="77">
         <v>34</v>
       </c>
-      <c r="G9" s="61">
+      <c r="G9" s="77">
+        <f t="shared" si="2"/>
         <v>21</v>
       </c>
-      <c r="H9" s="61">
+      <c r="H9" s="47">
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
-      <c r="I9" s="61">
+      <c r="I9" s="50">
         <v>48</v>
       </c>
-      <c r="J9" s="61">
+      <c r="J9" s="50">
         <v>-1.98</v>
       </c>
-      <c r="K9" s="61">
-        <v>18</v>
-      </c>
-      <c r="L9" s="61">
+      <c r="K9" s="50">
         <v>46.02</v>
       </c>
-      <c r="M9" s="61">
+      <c r="L9" s="50">
         <v>39.200000000000003</v>
       </c>
-      <c r="N9" s="75">
+      <c r="M9" s="64">
         <v>81.680000000000007</v>
       </c>
-      <c r="O9" s="61">
+      <c r="N9" s="50">
         <v>61.82</v>
       </c>
-      <c r="P9" s="61">
+      <c r="O9" s="50">
         <v>82</v>
       </c>
-      <c r="Q9" s="68">
+      <c r="P9" s="57">
         <v>203</v>
       </c>
-      <c r="R9" s="3">
+      <c r="Q9" s="3">
         <f t="shared" si="0"/>
         <v>60.098522167487687</v>
       </c>
-      <c r="T9" s="3">
+      <c r="R9" s="61" t="s">
+        <v>38</v>
+      </c>
+      <c r="S9" s="3">
         <f t="shared" si="1"/>
         <v>35.660000000000004</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A10" s="59"/>
-      <c r="B10" s="60">
+    <row r="10" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="48"/>
+      <c r="B10" s="49">
         <v>9</v>
       </c>
-      <c r="C10" s="85" t="s">
-        <v>26</v>
-      </c>
-      <c r="D10" s="85"/>
-      <c r="E10" s="61">
+      <c r="C10" s="70" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="70"/>
+      <c r="E10" s="77">
         <v>58</v>
       </c>
-      <c r="F10" s="61">
+      <c r="F10" s="77">
         <v>45</v>
       </c>
-      <c r="G10" s="61">
+      <c r="G10" s="77">
+        <f t="shared" si="2"/>
         <v>13</v>
       </c>
-      <c r="H10" s="61">
+      <c r="H10" s="47">
+        <f t="shared" si="3"/>
         <v>7</v>
       </c>
-      <c r="I10" s="61">
+      <c r="I10" s="50">
         <v>65</v>
       </c>
-      <c r="J10" s="61">
+      <c r="J10" s="50">
         <v>-5.28</v>
       </c>
-      <c r="K10" s="61">
-        <v>12</v>
-      </c>
-      <c r="L10" s="61">
+      <c r="K10" s="50">
         <v>59.72</v>
       </c>
-      <c r="M10" s="61">
+      <c r="L10" s="50">
         <v>42.88</v>
       </c>
-      <c r="N10" s="75">
+      <c r="M10" s="64">
         <v>86.02</v>
       </c>
-      <c r="O10" s="61">
+      <c r="N10" s="50">
         <v>77.59</v>
       </c>
-      <c r="P10" s="61">
+      <c r="O10" s="50">
         <v>43</v>
       </c>
-      <c r="Q10" s="68">
+      <c r="P10" s="57">
         <v>166</v>
       </c>
-      <c r="R10" s="3">
+      <c r="Q10" s="3">
         <f t="shared" si="0"/>
         <v>74.698795180722882</v>
       </c>
-      <c r="T10" s="3">
+      <c r="R10" s="61" t="s">
+        <v>38</v>
+      </c>
+      <c r="S10" s="3">
         <f t="shared" si="1"/>
         <v>26.299999999999997</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A11" s="59"/>
-      <c r="B11" s="60">
+    <row r="11" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="48"/>
+      <c r="B11" s="49">
         <v>10</v>
       </c>
-      <c r="C11" s="85" t="s">
-        <v>27</v>
-      </c>
-      <c r="D11" s="85"/>
-      <c r="E11" s="61">
+      <c r="C11" s="70" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="70"/>
+      <c r="E11" s="77">
         <v>60</v>
       </c>
-      <c r="F11" s="61">
+      <c r="F11" s="77">
         <v>42</v>
       </c>
-      <c r="G11" s="61">
+      <c r="G11" s="77">
+        <f t="shared" ref="G11:G38" si="4">E11-F11</f>
         <v>18</v>
       </c>
-      <c r="H11" s="61">
+      <c r="H11" s="47">
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
-      <c r="I11" s="61">
+      <c r="I11" s="50">
         <v>62</v>
       </c>
-      <c r="J11" s="61">
+      <c r="J11" s="50">
         <v>-4.62</v>
       </c>
-      <c r="K11" s="61">
-        <v>9</v>
-      </c>
-      <c r="L11" s="61">
+      <c r="K11" s="50">
         <v>57.38</v>
       </c>
-      <c r="M11" s="61">
+      <c r="L11" s="50">
         <v>43.61</v>
       </c>
-      <c r="N11" s="75">
+      <c r="M11" s="64">
         <v>83.02</v>
       </c>
-      <c r="O11" s="61">
+      <c r="N11" s="50">
         <v>70</v>
       </c>
-      <c r="P11" s="61">
+      <c r="O11" s="50">
         <v>171</v>
       </c>
-      <c r="Q11" s="68">
+      <c r="P11" s="57">
         <v>823</v>
       </c>
-      <c r="R11" s="3">
+      <c r="Q11" s="3">
         <f t="shared" si="0"/>
         <v>79.343863912515189</v>
       </c>
-      <c r="T11" s="3">
+      <c r="R11" s="61" t="s">
+        <v>38</v>
+      </c>
+      <c r="S11" s="3">
         <f t="shared" si="1"/>
         <v>25.639999999999993</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A12" s="59"/>
-      <c r="B12" s="60">
+    <row r="12" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="48"/>
+      <c r="B12" s="49">
         <v>11</v>
       </c>
-      <c r="C12" s="85" t="s">
-        <v>28</v>
-      </c>
-      <c r="D12" s="85"/>
-      <c r="E12" s="61">
+      <c r="C12" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="70"/>
+      <c r="E12" s="77">
         <v>56</v>
       </c>
-      <c r="F12" s="61">
+      <c r="F12" s="77">
         <v>42</v>
       </c>
-      <c r="G12" s="61">
+      <c r="G12" s="77">
+        <f t="shared" si="4"/>
         <v>14</v>
       </c>
-      <c r="H12" s="61">
+      <c r="H12" s="47">
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
-      <c r="I12" s="61">
+      <c r="I12" s="50">
         <v>62</v>
       </c>
-      <c r="J12" s="61">
+      <c r="J12" s="50">
         <v>-2.31</v>
       </c>
-      <c r="K12" s="61">
-        <v>17</v>
-      </c>
-      <c r="L12" s="61">
+      <c r="K12" s="50">
         <v>59.69</v>
       </c>
-      <c r="M12" s="61">
+      <c r="L12" s="50">
         <v>50.53</v>
       </c>
-      <c r="N12" s="75">
+      <c r="M12" s="64">
         <v>90</v>
       </c>
-      <c r="O12" s="61">
+      <c r="N12" s="50">
         <v>75</v>
       </c>
-      <c r="P12" s="61">
+      <c r="O12" s="50">
         <v>218</v>
       </c>
-      <c r="Q12" s="68">
+      <c r="P12" s="57">
         <v>616</v>
       </c>
-      <c r="R12" s="3">
+      <c r="Q12" s="3">
         <f t="shared" si="0"/>
         <v>64.772727272727266</v>
       </c>
-      <c r="T12" s="3">
+      <c r="R12" s="61" t="s">
+        <v>38</v>
+      </c>
+      <c r="S12" s="3">
         <f t="shared" si="1"/>
         <v>30.310000000000002</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A13" s="59"/>
-      <c r="B13" s="60">
+    <row r="13" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="48"/>
+      <c r="B13" s="49">
         <v>12</v>
       </c>
-      <c r="C13" s="85" t="s">
-        <v>29</v>
-      </c>
-      <c r="D13" s="85"/>
-      <c r="E13" s="61">
+      <c r="C13" s="70" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" s="70"/>
+      <c r="E13" s="77">
         <v>56</v>
       </c>
-      <c r="F13" s="61">
+      <c r="F13" s="77">
         <v>45</v>
       </c>
-      <c r="G13" s="61">
+      <c r="G13" s="77">
+        <f t="shared" si="4"/>
         <v>11</v>
       </c>
-      <c r="H13" s="61">
+      <c r="H13" s="47">
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
-      <c r="I13" s="61">
+      <c r="I13" s="50">
         <v>68</v>
       </c>
-      <c r="J13" s="61">
+      <c r="J13" s="50">
         <v>-3.3</v>
       </c>
-      <c r="K13" s="61">
-        <v>15</v>
-      </c>
-      <c r="L13" s="61">
+      <c r="K13" s="50">
         <v>64.7</v>
       </c>
-      <c r="M13" s="61">
+      <c r="L13" s="50">
         <v>52.6</v>
       </c>
-      <c r="N13" s="75">
+      <c r="M13" s="64">
         <v>89.34</v>
       </c>
-      <c r="O13" s="61">
+      <c r="N13" s="50">
         <v>80.36</v>
       </c>
-      <c r="P13" s="61">
+      <c r="O13" s="50">
         <v>141</v>
       </c>
-      <c r="Q13" s="68">
+      <c r="P13" s="57">
         <v>437</v>
       </c>
-      <c r="R13" s="3">
+      <c r="Q13" s="3">
         <f t="shared" si="0"/>
         <v>67.963386727688786</v>
       </c>
-      <c r="T13" s="3">
+      <c r="R13" s="61" t="s">
+        <v>38</v>
+      </c>
+      <c r="S13" s="3">
         <f t="shared" si="1"/>
         <v>24.64</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A14" s="59"/>
-      <c r="B14" s="60">
+    <row r="14" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="48"/>
+      <c r="B14" s="49">
         <v>13</v>
       </c>
-      <c r="C14" s="85" t="s">
-        <v>30</v>
-      </c>
-      <c r="D14" s="85"/>
-      <c r="E14" s="61">
+      <c r="C14" s="70" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14" s="70"/>
+      <c r="E14" s="77">
         <v>56</v>
       </c>
-      <c r="F14" s="61">
+      <c r="F14" s="77">
         <v>43</v>
       </c>
-      <c r="G14" s="61">
+      <c r="G14" s="77">
+        <f t="shared" si="4"/>
         <v>13</v>
       </c>
-      <c r="H14" s="61">
+      <c r="H14" s="47">
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
-      <c r="I14" s="61">
+      <c r="I14" s="50">
         <v>63</v>
       </c>
-      <c r="J14" s="61">
+      <c r="J14" s="50">
         <v>-2.64</v>
       </c>
-      <c r="K14" s="61">
-        <v>15</v>
-      </c>
-      <c r="L14" s="61">
+      <c r="K14" s="50">
         <v>60.36</v>
       </c>
-      <c r="M14" s="61">
+      <c r="L14" s="50">
         <v>46.4</v>
       </c>
-      <c r="N14" s="75">
+      <c r="M14" s="64">
         <v>84.35</v>
       </c>
-      <c r="O14" s="61">
+      <c r="N14" s="50">
         <v>76.790000000000006</v>
       </c>
-      <c r="P14" s="61">
+      <c r="O14" s="50">
         <v>114</v>
       </c>
-      <c r="Q14" s="68">
+      <c r="P14" s="57">
         <v>402</v>
       </c>
-      <c r="R14" s="3">
+      <c r="Q14" s="3">
         <f t="shared" si="0"/>
         <v>71.890547263681597</v>
       </c>
-      <c r="T14" s="3">
+      <c r="R14" s="61" t="s">
+        <v>38</v>
+      </c>
+      <c r="S14" s="3">
         <f t="shared" si="1"/>
         <v>23.989999999999995</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A15" s="59"/>
-      <c r="B15" s="60">
+    <row r="15" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="48"/>
+      <c r="B15" s="49">
         <v>14</v>
       </c>
-      <c r="C15" s="85" t="s">
-        <v>31</v>
-      </c>
-      <c r="D15" s="85"/>
-      <c r="E15" s="61">
+      <c r="C15" s="70" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" s="70"/>
+      <c r="E15" s="77">
         <v>50</v>
       </c>
-      <c r="F15" s="61">
+      <c r="F15" s="77">
         <v>40</v>
       </c>
-      <c r="G15" s="61">
+      <c r="G15" s="77">
+        <f t="shared" si="4"/>
         <v>10</v>
       </c>
-      <c r="H15" s="61">
+      <c r="H15" s="47">
+        <f t="shared" si="3"/>
         <v>15</v>
       </c>
-      <c r="I15" s="61">
+      <c r="I15" s="50">
         <v>65</v>
       </c>
-      <c r="J15" s="61">
+      <c r="J15" s="50">
         <v>-3</v>
       </c>
-      <c r="K15" s="61"/>
-      <c r="L15" s="61">
+      <c r="K15" s="50">
         <v>62</v>
       </c>
-      <c r="M15" s="61">
+      <c r="L15" s="50">
         <v>40.450000000000003</v>
       </c>
-      <c r="N15" s="75">
+      <c r="M15" s="64">
         <v>78.81</v>
       </c>
-      <c r="O15" s="61"/>
-      <c r="P15" s="61">
+      <c r="N15" s="50"/>
+      <c r="O15" s="50">
         <v>139</v>
       </c>
-      <c r="Q15" s="68">
+      <c r="P15" s="57">
         <v>100000</v>
       </c>
-      <c r="R15" s="3">
+      <c r="Q15" s="3">
         <f t="shared" si="0"/>
         <v>99.861999999999995</v>
       </c>
-      <c r="T15" s="3">
+      <c r="R15" s="61" t="s">
+        <v>38</v>
+      </c>
+      <c r="S15" s="3">
         <f t="shared" si="1"/>
         <v>16.810000000000002</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A16" s="59"/>
-      <c r="B16" s="60">
+    <row r="16" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="48"/>
+      <c r="B16" s="49">
         <v>15</v>
       </c>
-      <c r="C16" s="85" t="s">
-        <v>32</v>
-      </c>
-      <c r="D16" s="85"/>
-      <c r="E16" s="61">
+      <c r="C16" s="70" t="s">
+        <v>31</v>
+      </c>
+      <c r="D16" s="70"/>
+      <c r="E16" s="77">
         <v>56</v>
       </c>
-      <c r="F16" s="61">
+      <c r="F16" s="77">
         <v>50</v>
       </c>
-      <c r="G16" s="61">
+      <c r="G16" s="77">
+        <f t="shared" si="4"/>
         <v>6</v>
       </c>
-      <c r="H16" s="61">
+      <c r="H16" s="47">
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
-      <c r="I16" s="61">
+      <c r="I16" s="50">
         <v>71</v>
       </c>
-      <c r="J16" s="61">
+      <c r="J16" s="50">
         <v>-1.33</v>
       </c>
-      <c r="K16" s="61"/>
-      <c r="L16" s="61">
+      <c r="K16" s="50">
         <v>69.66</v>
       </c>
-      <c r="M16" s="61">
+      <c r="L16" s="50">
         <v>47.81</v>
       </c>
-      <c r="N16" s="75">
+      <c r="M16" s="64">
         <v>83.09</v>
       </c>
-      <c r="O16" s="61"/>
-      <c r="P16" s="61">
+      <c r="N16" s="50"/>
+      <c r="O16" s="50">
         <v>170</v>
       </c>
-      <c r="Q16" s="68">
+      <c r="P16" s="57">
         <v>100000</v>
       </c>
-      <c r="R16" s="3">
+      <c r="Q16" s="3">
         <f t="shared" si="0"/>
         <v>99.831000000000003</v>
       </c>
-      <c r="T16" s="3">
+      <c r="R16" s="61" t="s">
+        <v>38</v>
+      </c>
+      <c r="S16" s="3">
         <f t="shared" si="1"/>
         <v>13.430000000000007</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A17" s="59"/>
-      <c r="B17" s="60">
+    <row r="17" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="48"/>
+      <c r="B17" s="49">
         <v>16</v>
       </c>
-      <c r="C17" s="85" t="s">
-        <v>33</v>
-      </c>
-      <c r="D17" s="85"/>
-      <c r="E17" s="61">
+      <c r="C17" s="70" t="s">
+        <v>32</v>
+      </c>
+      <c r="D17" s="70"/>
+      <c r="E17" s="77">
         <v>53</v>
       </c>
-      <c r="F17" s="61">
+      <c r="F17" s="77">
         <v>43</v>
       </c>
-      <c r="G17" s="61">
+      <c r="G17" s="77">
+        <f t="shared" si="4"/>
         <v>10</v>
       </c>
-      <c r="H17" s="61">
+      <c r="H17" s="47">
+        <f t="shared" si="3"/>
         <v>12</v>
       </c>
-      <c r="I17" s="61">
+      <c r="I17" s="50">
         <v>64</v>
       </c>
-      <c r="J17" s="61">
+      <c r="J17" s="50">
         <v>-1.67</v>
       </c>
-      <c r="K17" s="61"/>
-      <c r="L17" s="61">
+      <c r="K17" s="50">
         <v>62.33</v>
       </c>
-      <c r="M17" s="61">
+      <c r="L17" s="50">
         <v>43.84</v>
       </c>
-      <c r="N17" s="75">
+      <c r="M17" s="64">
         <v>82.46</v>
       </c>
-      <c r="O17" s="61"/>
-      <c r="P17" s="61">
+      <c r="N17" s="50"/>
+      <c r="O17" s="50">
         <v>201</v>
       </c>
-      <c r="Q17" s="68">
+      <c r="P17" s="57">
         <v>150000</v>
       </c>
-      <c r="R17" s="3">
+      <c r="Q17" s="3">
         <f t="shared" si="0"/>
         <v>99.866666666666674</v>
       </c>
-      <c r="T17" s="3">
+      <c r="R17" s="61" t="s">
+        <v>38</v>
+      </c>
+      <c r="S17" s="3">
         <f t="shared" si="1"/>
         <v>20.129999999999995</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A18" s="59"/>
-      <c r="B18" s="60">
+    <row r="18" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="48"/>
+      <c r="B18" s="49">
         <v>17</v>
       </c>
-      <c r="C18" s="85" t="s">
-        <v>34</v>
-      </c>
-      <c r="D18" s="85"/>
-      <c r="E18" s="61">
+      <c r="C18" s="70" t="s">
+        <v>33</v>
+      </c>
+      <c r="D18" s="70"/>
+      <c r="E18" s="77">
         <v>58</v>
       </c>
-      <c r="F18" s="61">
+      <c r="F18" s="77">
         <v>41</v>
       </c>
-      <c r="G18" s="61">
+      <c r="G18" s="77">
+        <f t="shared" si="4"/>
         <v>17</v>
       </c>
-      <c r="H18" s="61">
+      <c r="H18" s="47">
+        <f t="shared" si="3"/>
         <v>7</v>
       </c>
-      <c r="I18" s="61">
+      <c r="I18" s="50">
         <v>62</v>
       </c>
-      <c r="J18" s="61">
+      <c r="J18" s="50">
         <v>-2.97</v>
       </c>
-      <c r="K18" s="61">
-        <v>13</v>
-      </c>
-      <c r="L18" s="61">
+      <c r="K18" s="50">
         <v>59.03</v>
       </c>
-      <c r="M18" s="61">
+      <c r="L18" s="50">
         <v>48.22</v>
       </c>
-      <c r="N18" s="75">
+      <c r="M18" s="64">
         <v>88.68</v>
       </c>
-      <c r="O18" s="61">
+      <c r="N18" s="50">
         <v>70.69</v>
       </c>
-      <c r="P18" s="61">
+      <c r="O18" s="50">
         <v>397</v>
       </c>
-      <c r="Q18" s="68">
+      <c r="P18" s="57">
         <v>1335</v>
       </c>
-      <c r="R18" s="3">
+      <c r="Q18" s="3">
         <f t="shared" si="0"/>
         <v>70.337078651685388</v>
       </c>
-      <c r="T18" s="3">
+      <c r="R18" s="61" t="s">
+        <v>38</v>
+      </c>
+      <c r="S18" s="3">
         <f t="shared" si="1"/>
         <v>29.650000000000006</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A19" s="59"/>
-      <c r="B19" s="60">
+    <row r="19" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="48"/>
+      <c r="B19" s="49">
         <v>18</v>
       </c>
-      <c r="C19" s="85" t="s">
-        <v>35</v>
-      </c>
-      <c r="D19" s="85"/>
-      <c r="E19" s="61">
+      <c r="C19" s="70" t="s">
+        <v>34</v>
+      </c>
+      <c r="D19" s="70"/>
+      <c r="E19" s="77">
         <v>60</v>
       </c>
-      <c r="F19" s="61">
+      <c r="F19" s="77">
         <v>51</v>
       </c>
-      <c r="G19" s="61">
+      <c r="G19" s="77">
+        <f t="shared" si="4"/>
         <v>9</v>
       </c>
-      <c r="H19" s="61">
+      <c r="H19" s="47">
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
-      <c r="I19" s="61">
+      <c r="I19" s="50">
         <v>79</v>
       </c>
-      <c r="J19" s="61">
+      <c r="J19" s="50">
         <v>-1.32</v>
       </c>
-      <c r="K19" s="61">
-        <v>8</v>
-      </c>
-      <c r="L19" s="61">
+      <c r="K19" s="50">
         <v>77.680000000000007</v>
       </c>
-      <c r="M19" s="61">
+      <c r="L19" s="50">
         <v>49.92</v>
       </c>
-      <c r="N19" s="75">
+      <c r="M19" s="64">
         <v>86.68</v>
       </c>
-      <c r="O19" s="61">
+      <c r="N19" s="50">
         <v>85</v>
       </c>
-      <c r="P19" s="61">
+      <c r="O19" s="50">
         <v>31</v>
       </c>
-      <c r="Q19" s="68">
+      <c r="P19" s="57">
         <v>1315</v>
       </c>
-      <c r="R19" s="3">
+      <c r="Q19" s="3">
         <f t="shared" si="0"/>
         <v>97.718631178707227</v>
       </c>
-      <c r="T19" s="3">
+      <c r="R19" s="61" t="s">
+        <v>38</v>
+      </c>
+      <c r="S19" s="3">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A20" s="59"/>
-      <c r="B20" s="60">
+    <row r="20" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="48"/>
+      <c r="B20" s="49">
         <v>19</v>
       </c>
-      <c r="C20" s="85" t="s">
-        <v>36</v>
-      </c>
-      <c r="D20" s="85"/>
-      <c r="E20" s="61">
+      <c r="C20" s="70" t="s">
+        <v>35</v>
+      </c>
+      <c r="D20" s="70"/>
+      <c r="E20" s="77">
         <v>59</v>
       </c>
-      <c r="F20" s="61">
+      <c r="F20" s="77">
         <v>44</v>
       </c>
-      <c r="G20" s="61">
+      <c r="G20" s="77">
+        <f t="shared" si="4"/>
         <v>15</v>
       </c>
-      <c r="H20" s="61">
+      <c r="H20" s="47">
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
-      <c r="I20" s="61">
+      <c r="I20" s="50">
         <v>67</v>
       </c>
-      <c r="J20" s="61">
+      <c r="J20" s="50">
         <v>-2.64</v>
       </c>
-      <c r="K20" s="61">
-        <v>11</v>
-      </c>
-      <c r="L20" s="61">
+      <c r="K20" s="50">
         <v>64.36</v>
       </c>
-      <c r="M20" s="61">
+      <c r="L20" s="50">
         <v>46.71</v>
       </c>
-      <c r="N20" s="75">
+      <c r="M20" s="64">
         <v>83</v>
       </c>
-      <c r="O20" s="61">
+      <c r="N20" s="50">
         <v>74.58</v>
       </c>
-      <c r="P20" s="61">
+      <c r="O20" s="50">
         <v>137</v>
       </c>
-      <c r="Q20" s="68">
+      <c r="P20" s="57">
         <v>865</v>
       </c>
-      <c r="R20" s="3">
+      <c r="Q20" s="3">
         <f t="shared" si="0"/>
         <v>84.277456647398836</v>
       </c>
-      <c r="T20" s="3">
+      <c r="R20" s="61" t="s">
+        <v>38</v>
+      </c>
+      <c r="S20" s="3">
         <f t="shared" si="1"/>
         <v>18.64</v>
       </c>
     </row>
-    <row r="21" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="62"/>
-      <c r="B21" s="63">
+    <row r="21" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="51"/>
+      <c r="B21" s="52">
         <v>20</v>
       </c>
-      <c r="C21" s="88" t="s">
-        <v>37</v>
-      </c>
-      <c r="D21" s="88"/>
-      <c r="E21" s="64">
+      <c r="C21" s="74" t="s">
+        <v>36</v>
+      </c>
+      <c r="D21" s="74"/>
+      <c r="E21" s="78">
         <v>56</v>
       </c>
-      <c r="F21" s="64">
+      <c r="F21" s="78">
         <v>43</v>
       </c>
-      <c r="G21" s="64">
+      <c r="G21" s="77">
+        <f t="shared" si="4"/>
         <v>13</v>
       </c>
-      <c r="H21" s="64">
+      <c r="H21" s="47">
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
-      <c r="I21" s="64">
+      <c r="I21" s="53">
         <v>64</v>
       </c>
-      <c r="J21" s="64">
+      <c r="J21" s="53">
         <v>-3.3</v>
       </c>
-      <c r="K21" s="64">
-        <v>15</v>
-      </c>
-      <c r="L21" s="64">
+      <c r="K21" s="53">
         <v>60.7</v>
       </c>
-      <c r="M21" s="64">
+      <c r="L21" s="53">
         <v>41.19</v>
       </c>
-      <c r="N21" s="76">
+      <c r="M21" s="65">
         <v>82.02</v>
       </c>
-      <c r="O21" s="64">
+      <c r="N21" s="53">
         <v>76.790000000000006</v>
       </c>
-      <c r="P21" s="64">
+      <c r="O21" s="53">
         <v>120</v>
       </c>
-      <c r="Q21" s="69">
+      <c r="P21" s="58">
         <v>826</v>
       </c>
-      <c r="R21" s="3">
+      <c r="Q21" s="3">
         <f t="shared" si="0"/>
         <v>85.593220338983059</v>
       </c>
-      <c r="T21" s="3">
+      <c r="R21" s="61" t="s">
+        <v>38</v>
+      </c>
+      <c r="S21" s="3">
         <f t="shared" si="1"/>
         <v>21.319999999999993</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A22" s="44">
+    <row r="22" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="39">
         <v>44808</v>
       </c>
-      <c r="B22" s="45">
+      <c r="B22" s="84">
         <v>21</v>
       </c>
-      <c r="C22" s="89" t="s">
+      <c r="C22" s="85" t="s">
+        <v>37</v>
+      </c>
+      <c r="D22" s="86"/>
+      <c r="E22" s="79">
+        <v>57</v>
+      </c>
+      <c r="F22" s="80">
+        <v>43</v>
+      </c>
+      <c r="G22" s="77">
+        <f t="shared" si="4"/>
+        <v>14</v>
+      </c>
+      <c r="H22" s="47">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+      <c r="I22" s="40">
+        <v>64</v>
+      </c>
+      <c r="J22" s="41">
+        <v>-3.96</v>
+      </c>
+      <c r="K22" s="42">
+        <v>60.04</v>
+      </c>
+      <c r="L22" s="43">
+        <v>9.25</v>
+      </c>
+      <c r="M22" s="66">
+        <v>76.36</v>
+      </c>
+      <c r="N22" s="44">
+        <v>75.44</v>
+      </c>
+      <c r="O22" s="40">
+        <v>11</v>
+      </c>
+      <c r="P22" s="59">
+        <v>595</v>
+      </c>
+      <c r="Q22" s="3">
+        <f t="shared" ref="Q22:Q39" si="5" xml:space="preserve"> (P22-O22+1)/(P22)*100</f>
+        <v>98.319327731092429</v>
+      </c>
+      <c r="R22" s="61" t="s">
         <v>38</v>
       </c>
-      <c r="D22" s="90"/>
-      <c r="E22" s="46">
-        <v>57</v>
-      </c>
-      <c r="F22" s="47">
-        <v>43</v>
-      </c>
-      <c r="G22" s="48">
-        <v>14</v>
-      </c>
-      <c r="H22" s="49">
-        <v>8</v>
-      </c>
-      <c r="I22" s="50">
-        <v>64</v>
-      </c>
-      <c r="J22" s="51">
-        <v>-3.96</v>
-      </c>
-      <c r="K22" s="52">
-        <v>15</v>
-      </c>
-      <c r="L22" s="53">
-        <v>60.04</v>
-      </c>
-      <c r="M22" s="54">
-        <v>9.25</v>
-      </c>
-      <c r="N22" s="77">
-        <v>76.36</v>
-      </c>
-      <c r="O22" s="55">
-        <v>75.44</v>
-      </c>
-      <c r="P22" s="50">
-        <v>11</v>
-      </c>
-      <c r="Q22" s="70">
-        <v>595</v>
-      </c>
-      <c r="R22" s="3">
-        <f t="shared" ref="R22:R39" si="2" xml:space="preserve"> (Q22-P22+1)/(Q22)*100</f>
-        <v>98.319327731092429</v>
-      </c>
-      <c r="S22" s="72" t="s">
-        <v>39</v>
-      </c>
-      <c r="T22" s="3">
+      <c r="S22" s="3">
         <f t="shared" si="1"/>
         <v>16.32</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A23" s="31">
+    <row r="23" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="28">
         <v>44816</v>
       </c>
-      <c r="B23" s="3">
+      <c r="B23" s="87">
         <v>22</v>
       </c>
-      <c r="C23" s="81" t="s">
-        <v>40</v>
-      </c>
-      <c r="D23" s="82"/>
-      <c r="E23" s="12">
+      <c r="C23" s="88" t="s">
+        <v>39</v>
+      </c>
+      <c r="D23" s="89"/>
+      <c r="E23" s="81">
         <v>58</v>
       </c>
-      <c r="F23" s="13">
+      <c r="F23" s="82">
         <v>44</v>
       </c>
-      <c r="G23" s="14">
+      <c r="G23" s="77">
+        <f t="shared" si="4"/>
         <v>14</v>
       </c>
-      <c r="H23" s="32">
+      <c r="H23" s="47">
+        <f t="shared" si="3"/>
         <v>7</v>
       </c>
-      <c r="I23" s="19">
+      <c r="I23" s="16">
         <v>66</v>
       </c>
-      <c r="J23" s="28">
+      <c r="J23" s="25">
         <v>-1.65</v>
       </c>
-      <c r="K23" s="33">
-        <v>14</v>
-      </c>
-      <c r="L23" s="16">
+      <c r="K23" s="13">
         <v>64.349999999999994</v>
       </c>
-      <c r="M23" s="17">
+      <c r="L23" s="14">
         <v>30.77</v>
       </c>
-      <c r="N23" s="75">
+      <c r="M23" s="64">
         <v>73.34</v>
       </c>
-      <c r="O23" s="18">
+      <c r="N23" s="15">
         <v>75.86</v>
       </c>
-      <c r="P23" s="19">
+      <c r="O23" s="16">
         <v>10</v>
       </c>
-      <c r="Q23" s="71">
+      <c r="P23" s="60">
         <v>88</v>
       </c>
-      <c r="R23" s="3">
-        <f t="shared" si="2"/>
+      <c r="Q23" s="3">
+        <f t="shared" si="5"/>
         <v>89.772727272727266</v>
       </c>
-      <c r="S23" s="72" t="s">
-        <v>39</v>
-      </c>
-      <c r="T23" s="3">
+      <c r="R23" s="61" t="s">
+        <v>38</v>
+      </c>
+      <c r="S23" s="3">
         <f t="shared" si="1"/>
         <v>8.9900000000000091</v>
       </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A24" s="31">
+    <row r="24" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="28">
         <v>44822</v>
       </c>
-      <c r="B24" s="3">
+      <c r="B24" s="87">
         <v>23</v>
       </c>
-      <c r="C24" s="81" t="s">
-        <v>41</v>
-      </c>
-      <c r="D24" s="82"/>
-      <c r="E24" s="12">
+      <c r="C24" s="88" t="s">
+        <v>40</v>
+      </c>
+      <c r="D24" s="89"/>
+      <c r="E24" s="81">
         <v>64</v>
       </c>
-      <c r="F24" s="13">
+      <c r="F24" s="82">
         <v>46</v>
       </c>
-      <c r="G24" s="14">
+      <c r="G24" s="77">
+        <f t="shared" si="4"/>
         <v>18</v>
       </c>
-      <c r="H24" s="32">
+      <c r="H24" s="47">
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="I24" s="19">
+      <c r="I24" s="16">
         <v>71</v>
       </c>
-      <c r="J24" s="28">
+      <c r="J24" s="25">
         <v>-2.97</v>
       </c>
-      <c r="K24" s="33">
-        <v>2</v>
-      </c>
-      <c r="L24" s="16">
+      <c r="K24" s="13">
         <v>68.03</v>
       </c>
-      <c r="M24" s="17">
+      <c r="L24" s="14">
         <v>26.27</v>
       </c>
-      <c r="N24" s="75">
+      <c r="M24" s="64">
         <v>77.680000000000007</v>
       </c>
-      <c r="O24" s="18">
+      <c r="N24" s="15">
         <v>71.88</v>
       </c>
-      <c r="P24" s="19">
+      <c r="O24" s="16">
         <v>6</v>
       </c>
-      <c r="Q24" s="71">
+      <c r="P24" s="60">
         <v>52</v>
       </c>
-      <c r="R24" s="3">
-        <f t="shared" si="2"/>
+      <c r="Q24" s="3">
+        <f t="shared" si="5"/>
         <v>90.384615384615387</v>
       </c>
-      <c r="S24" s="72" t="s">
-        <v>39</v>
-      </c>
-      <c r="T24" s="3">
+      <c r="R24" s="61" t="s">
+        <v>38</v>
+      </c>
+      <c r="S24" s="3">
         <f t="shared" si="1"/>
         <v>9.6500000000000057</v>
       </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A25" s="31">
+    <row r="25" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="28">
         <v>44857</v>
       </c>
-      <c r="B25" s="3">
+      <c r="B25" s="87">
         <v>24</v>
       </c>
-      <c r="C25" s="81" t="s">
-        <v>42</v>
-      </c>
-      <c r="D25" s="82"/>
-      <c r="E25" s="12">
+      <c r="C25" s="88" t="s">
+        <v>41</v>
+      </c>
+      <c r="D25" s="89"/>
+      <c r="E25" s="81">
         <v>63</v>
       </c>
-      <c r="F25" s="13">
+      <c r="F25" s="82">
         <v>45</v>
       </c>
-      <c r="G25" s="14">
+      <c r="G25" s="77">
+        <f t="shared" si="4"/>
         <v>18</v>
       </c>
-      <c r="H25" s="32">
+      <c r="H25" s="47">
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
-      <c r="I25" s="19">
+      <c r="I25" s="16">
         <v>65</v>
       </c>
-      <c r="J25" s="28">
+      <c r="J25" s="25">
         <v>-3.3</v>
       </c>
-      <c r="K25" s="33">
+      <c r="K25" s="13">
+        <v>61.7</v>
+      </c>
+      <c r="L25" s="14">
+        <v>35.83</v>
+      </c>
+      <c r="M25" s="64">
+        <v>62.03</v>
+      </c>
+      <c r="N25" s="15">
+        <v>71.430000000000007</v>
+      </c>
+      <c r="O25" s="16">
         <v>3</v>
       </c>
-      <c r="L25" s="16">
-        <v>61.7</v>
-      </c>
-      <c r="M25" s="17">
-        <v>35.83</v>
-      </c>
-      <c r="N25" s="75">
-        <v>62.03</v>
-      </c>
-      <c r="O25" s="18">
-        <v>71.430000000000007</v>
-      </c>
-      <c r="P25" s="19">
-        <v>3</v>
-      </c>
-      <c r="Q25" s="71">
+      <c r="P25" s="60">
         <v>26</v>
       </c>
-      <c r="R25" s="3">
-        <f t="shared" si="2"/>
+      <c r="Q25" s="3">
+        <f t="shared" si="5"/>
         <v>92.307692307692307</v>
       </c>
-      <c r="S25" s="72" t="s">
-        <v>39</v>
-      </c>
-      <c r="T25" s="3">
+      <c r="R25" s="61" t="s">
+        <v>38</v>
+      </c>
+      <c r="S25" s="3">
         <f t="shared" si="1"/>
         <v>0.32999999999999829</v>
       </c>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A26" s="31">
+    <row r="26" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="28">
         <v>44871</v>
       </c>
-      <c r="B26" s="3">
+      <c r="B26" s="87">
         <v>25</v>
       </c>
-      <c r="C26" s="81" t="s">
-        <v>43</v>
-      </c>
-      <c r="D26" s="82"/>
-      <c r="E26" s="12">
+      <c r="C26" s="88" t="s">
+        <v>42</v>
+      </c>
+      <c r="D26" s="89"/>
+      <c r="E26" s="81">
         <v>63</v>
       </c>
-      <c r="F26" s="13">
+      <c r="F26" s="82">
         <v>45</v>
       </c>
-      <c r="G26" s="14">
+      <c r="G26" s="77">
+        <f t="shared" si="4"/>
         <v>18</v>
       </c>
-      <c r="H26" s="32">
+      <c r="H26" s="47">
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
-      <c r="I26" s="19">
+      <c r="I26" s="16">
         <v>69</v>
       </c>
-      <c r="J26" s="28">
+      <c r="J26" s="25">
         <v>-2.64</v>
       </c>
-      <c r="K26" s="33">
-        <v>3</v>
-      </c>
-      <c r="L26" s="16">
+      <c r="K26" s="13">
         <v>66.36</v>
       </c>
-      <c r="M26" s="17">
+      <c r="L26" s="14">
         <v>47.2</v>
       </c>
-      <c r="N26" s="75">
+      <c r="M26" s="64">
         <v>75.02</v>
       </c>
-      <c r="O26" s="18">
+      <c r="N26" s="15">
         <v>71.430000000000007</v>
       </c>
-      <c r="P26" s="19">
+      <c r="O26" s="16">
         <v>7</v>
       </c>
-      <c r="Q26" s="71">
+      <c r="P26" s="60">
         <v>40</v>
       </c>
-      <c r="R26" s="3">
-        <f t="shared" si="2"/>
+      <c r="Q26" s="3">
+        <f t="shared" si="5"/>
         <v>85</v>
       </c>
-      <c r="S26" s="72" t="s">
-        <v>39</v>
-      </c>
-      <c r="T26" s="3">
+      <c r="R26" s="61" t="s">
+        <v>38</v>
+      </c>
+      <c r="S26" s="3">
         <f t="shared" si="1"/>
         <v>8.6599999999999966</v>
       </c>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A27" s="31">
+    <row r="27" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="28">
         <v>44874</v>
       </c>
-      <c r="B27" s="3">
+      <c r="B27" s="87">
         <v>26</v>
       </c>
-      <c r="C27" s="81" t="s">
-        <v>44</v>
-      </c>
-      <c r="D27" s="82"/>
-      <c r="E27" s="12">
+      <c r="C27" s="88" t="s">
+        <v>43</v>
+      </c>
+      <c r="D27" s="89"/>
+      <c r="E27" s="81">
         <v>61</v>
       </c>
-      <c r="F27" s="13">
+      <c r="F27" s="82">
         <v>42</v>
       </c>
-      <c r="G27" s="14">
+      <c r="G27" s="77">
+        <f t="shared" si="4"/>
         <v>19</v>
       </c>
-      <c r="H27" s="32">
+      <c r="H27" s="47">
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
-      <c r="I27" s="19">
+      <c r="I27" s="16">
         <v>62</v>
       </c>
-      <c r="J27" s="28">
+      <c r="J27" s="25">
         <v>-0.99</v>
       </c>
-      <c r="K27" s="33">
-        <v>5</v>
-      </c>
-      <c r="L27" s="16">
+      <c r="K27" s="13">
         <v>61.01</v>
       </c>
-      <c r="M27" s="17">
+      <c r="L27" s="14">
         <v>44.62</v>
       </c>
-      <c r="N27" s="17">
+      <c r="M27" s="14">
         <v>75.010000000000005</v>
       </c>
-      <c r="O27" s="18">
+      <c r="N27" s="15">
         <v>68.849999999999994</v>
       </c>
-      <c r="P27" s="19">
+      <c r="O27" s="16">
         <v>8</v>
       </c>
-      <c r="Q27" s="19">
+      <c r="P27" s="16">
         <v>46</v>
       </c>
-      <c r="R27" s="3">
-        <f t="shared" si="2"/>
+      <c r="Q27" s="3">
+        <f t="shared" si="5"/>
         <v>84.782608695652172</v>
       </c>
-      <c r="S27" s="72" t="s">
-        <v>39</v>
-      </c>
-      <c r="T27" s="3">
+      <c r="R27" s="61" t="s">
+        <v>38</v>
+      </c>
+      <c r="S27" s="3">
         <f t="shared" si="1"/>
         <v>14.000000000000007</v>
       </c>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A28" s="31">
+    <row r="28" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="28">
         <v>44878</v>
       </c>
-      <c r="B28" s="3">
+      <c r="B28" s="87">
         <v>27</v>
       </c>
-      <c r="C28" s="83" t="s">
-        <v>45</v>
-      </c>
-      <c r="D28" s="83"/>
-      <c r="E28" s="12">
+      <c r="C28" s="90" t="s">
+        <v>44</v>
+      </c>
+      <c r="D28" s="90"/>
+      <c r="E28" s="81">
         <v>65</v>
       </c>
-      <c r="F28" s="13">
+      <c r="F28" s="82">
         <v>56</v>
       </c>
-      <c r="G28" s="14">
+      <c r="G28" s="77">
+        <f t="shared" si="4"/>
         <v>9</v>
       </c>
-      <c r="H28" s="32">
+      <c r="H28" s="47">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="I28" s="19">
+      <c r="I28" s="16">
         <v>85</v>
       </c>
-      <c r="J28" s="28">
+      <c r="J28" s="25">
         <v>-1.65</v>
       </c>
-      <c r="K28" s="33">
-        <v>0</v>
-      </c>
-      <c r="L28" s="16">
+      <c r="K28" s="13">
         <v>83.35</v>
       </c>
-      <c r="M28" s="17">
+      <c r="L28" s="14">
         <v>45.78</v>
       </c>
-      <c r="N28" s="17">
+      <c r="M28" s="14">
         <v>83.35</v>
       </c>
-      <c r="O28" s="18">
+      <c r="N28" s="15">
         <v>86.15</v>
       </c>
-      <c r="P28" s="19">
+      <c r="O28" s="16">
         <v>1</v>
       </c>
-      <c r="Q28" s="19">
+      <c r="P28" s="16">
         <v>34</v>
       </c>
-      <c r="R28" s="3">
-        <f t="shared" si="2"/>
+      <c r="Q28" s="3">
+        <f t="shared" si="5"/>
         <v>100</v>
       </c>
-      <c r="S28" s="72" t="s">
-        <v>39</v>
-      </c>
-      <c r="T28" s="3">
+      <c r="R28" s="61" t="s">
+        <v>38</v>
+      </c>
+      <c r="S28" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A29" s="31"/>
-      <c r="B29" s="3">
+    <row r="29" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="28"/>
+      <c r="B29" s="91">
         <v>28</v>
       </c>
-      <c r="C29" s="81" t="s">
-        <v>46</v>
-      </c>
-      <c r="D29" s="82"/>
-      <c r="E29" s="12"/>
-      <c r="F29" s="13"/>
-      <c r="G29" s="14"/>
-      <c r="H29" s="32"/>
-      <c r="I29" s="19"/>
-      <c r="J29" s="28"/>
-      <c r="K29" s="33"/>
-      <c r="L29" s="16"/>
-      <c r="M29" s="17"/>
-      <c r="N29" s="75"/>
-      <c r="O29" s="18"/>
-      <c r="P29" s="19"/>
-      <c r="Q29" s="71"/>
-      <c r="R29" s="3" t="e">
-        <f t="shared" si="2"/>
+      <c r="C29" s="92" t="s">
+        <v>45</v>
+      </c>
+      <c r="D29" s="93"/>
+      <c r="E29" s="81"/>
+      <c r="F29" s="82"/>
+      <c r="G29" s="77">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="H29" s="47"/>
+      <c r="I29" s="16"/>
+      <c r="J29" s="25"/>
+      <c r="K29" s="13"/>
+      <c r="L29" s="14"/>
+      <c r="M29" s="64"/>
+      <c r="N29" s="15"/>
+      <c r="O29" s="16"/>
+      <c r="P29" s="60"/>
+      <c r="Q29" s="3" t="e">
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="S29" s="72"/>
-      <c r="T29" s="3">
+      <c r="R29" s="61"/>
+      <c r="S29" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A30" s="31"/>
-      <c r="B30" s="3">
+    <row r="30" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="28">
+        <v>44881</v>
+      </c>
+      <c r="B30" s="87">
         <v>29</v>
       </c>
-      <c r="C30" s="81" t="s">
+      <c r="C30" s="88" t="s">
+        <v>46</v>
+      </c>
+      <c r="D30" s="89"/>
+      <c r="E30" s="81">
+        <v>63</v>
+      </c>
+      <c r="F30" s="82">
+        <v>51</v>
+      </c>
+      <c r="G30" s="77">
+        <f t="shared" si="4"/>
+        <v>12</v>
+      </c>
+      <c r="H30" s="47">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="I30" s="16">
+        <v>77</v>
+      </c>
+      <c r="J30" s="25">
+        <v>-2.31</v>
+      </c>
+      <c r="K30" s="13">
+        <v>74.69</v>
+      </c>
+      <c r="L30" s="14">
+        <v>45.83</v>
+      </c>
+      <c r="M30" s="64">
+        <v>86</v>
+      </c>
+      <c r="N30" s="15">
+        <v>80.95</v>
+      </c>
+      <c r="O30" s="16">
+        <v>7</v>
+      </c>
+      <c r="P30" s="60">
+        <v>122</v>
+      </c>
+      <c r="Q30" s="3">
+        <f t="shared" si="5"/>
+        <v>95.081967213114751</v>
+      </c>
+      <c r="R30" s="61" t="s">
+        <v>38</v>
+      </c>
+      <c r="S30" s="3">
+        <f t="shared" si="1"/>
+        <v>11.310000000000002</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="28">
+        <v>44915</v>
+      </c>
+      <c r="B31" s="87">
+        <v>30</v>
+      </c>
+      <c r="C31" s="88" t="s">
+        <v>53</v>
+      </c>
+      <c r="D31" s="89"/>
+      <c r="E31" s="81">
+        <v>55</v>
+      </c>
+      <c r="F31" s="82">
+        <v>41</v>
+      </c>
+      <c r="G31" s="77">
+        <f t="shared" si="4"/>
+        <v>14</v>
+      </c>
+      <c r="H31" s="47">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+      <c r="I31" s="16">
+        <v>61</v>
+      </c>
+      <c r="J31" s="25">
+        <v>-3.67</v>
+      </c>
+      <c r="K31" s="13">
+        <v>59.33</v>
+      </c>
+      <c r="L31" s="14"/>
+      <c r="M31" s="64">
+        <v>81</v>
+      </c>
+      <c r="N31" s="15"/>
+      <c r="O31" s="16">
+        <v>30</v>
+      </c>
+      <c r="P31" s="60">
+        <v>113</v>
+      </c>
+      <c r="Q31" s="3">
+        <f t="shared" si="5"/>
+        <v>74.336283185840713</v>
+      </c>
+      <c r="R31" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="S31" s="3">
+        <f t="shared" si="1"/>
+        <v>21.67</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="28">
+        <v>44917</v>
+      </c>
+      <c r="B32" s="87">
+        <v>31</v>
+      </c>
+      <c r="C32" s="88" t="s">
+        <v>54</v>
+      </c>
+      <c r="D32" s="89"/>
+      <c r="E32" s="81">
+        <v>52</v>
+      </c>
+      <c r="F32" s="82">
+        <v>37</v>
+      </c>
+      <c r="G32" s="77">
+        <f t="shared" si="4"/>
+        <v>15</v>
+      </c>
+      <c r="H32" s="47">
+        <f t="shared" si="3"/>
+        <v>13</v>
+      </c>
+      <c r="I32" s="16">
+        <v>55</v>
+      </c>
+      <c r="J32" s="25">
+        <v>-3</v>
+      </c>
+      <c r="K32" s="13">
+        <v>52</v>
+      </c>
+      <c r="L32" s="14"/>
+      <c r="M32" s="64">
+        <v>81</v>
+      </c>
+      <c r="N32" s="15"/>
+      <c r="O32" s="16"/>
+      <c r="P32" s="60"/>
+      <c r="Q32" s="3" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R32" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="S32" s="3">
+        <f t="shared" si="1"/>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="28">
+        <v>44925</v>
+      </c>
+      <c r="B33" s="87">
+        <v>32</v>
+      </c>
+      <c r="C33" s="88" t="s">
+        <v>55</v>
+      </c>
+      <c r="D33" s="89"/>
+      <c r="E33" s="81">
+        <v>58</v>
+      </c>
+      <c r="F33" s="82">
+        <v>48</v>
+      </c>
+      <c r="G33" s="77">
+        <f t="shared" si="4"/>
+        <v>10</v>
+      </c>
+      <c r="H33" s="47">
+        <f t="shared" si="3"/>
+        <v>7</v>
+      </c>
+      <c r="I33" s="16">
+        <v>71</v>
+      </c>
+      <c r="J33" s="25">
+        <v>-1</v>
+      </c>
+      <c r="K33" s="13">
+        <v>70</v>
+      </c>
+      <c r="L33" s="14">
+        <v>44.97</v>
+      </c>
+      <c r="M33" s="64">
+        <v>79</v>
+      </c>
+      <c r="N33" s="15"/>
+      <c r="O33" s="16">
+        <v>6</v>
+      </c>
+      <c r="P33" s="60">
+        <v>68</v>
+      </c>
+      <c r="Q33" s="3">
+        <f t="shared" si="5"/>
+        <v>92.64705882352942</v>
+      </c>
+      <c r="R33" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="S33" s="3">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="28">
+        <v>44928</v>
+      </c>
+      <c r="B34" s="87">
+        <v>33</v>
+      </c>
+      <c r="C34" s="88" t="s">
+        <v>56</v>
+      </c>
+      <c r="D34" s="89"/>
+      <c r="E34" s="81">
+        <v>57</v>
+      </c>
+      <c r="F34" s="82">
+        <v>48</v>
+      </c>
+      <c r="G34" s="77">
+        <f t="shared" si="4"/>
+        <v>9</v>
+      </c>
+      <c r="H34" s="47">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+      <c r="I34" s="16">
+        <v>73</v>
+      </c>
+      <c r="J34" s="25">
+        <v>-2.33</v>
+      </c>
+      <c r="K34" s="13">
+        <v>70.66</v>
+      </c>
+      <c r="L34" s="14">
+        <v>40.619999999999997</v>
+      </c>
+      <c r="M34" s="64">
+        <v>71.33</v>
+      </c>
+      <c r="N34" s="15"/>
+      <c r="O34" s="16">
+        <v>2</v>
+      </c>
+      <c r="P34" s="60">
+        <v>43</v>
+      </c>
+      <c r="Q34" s="3">
+        <f t="shared" si="5"/>
+        <v>97.674418604651152</v>
+      </c>
+      <c r="R34" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="S34" s="3">
+        <f t="shared" si="1"/>
+        <v>0.67000000000000171</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="28"/>
+      <c r="B35" s="3">
+        <v>30</v>
+      </c>
+      <c r="C35" s="75" t="s">
         <v>47</v>
       </c>
-      <c r="D30" s="82"/>
-      <c r="E30" s="12"/>
-      <c r="F30" s="13"/>
-      <c r="G30" s="14"/>
-      <c r="H30" s="32"/>
-      <c r="I30" s="19"/>
-      <c r="J30" s="28"/>
-      <c r="K30" s="33"/>
-      <c r="L30" s="16"/>
-      <c r="M30" s="17"/>
-      <c r="N30" s="75"/>
-      <c r="O30" s="18"/>
-      <c r="P30" s="19"/>
-      <c r="Q30" s="71"/>
-      <c r="R30" s="3" t="e">
-        <f t="shared" si="2"/>
+      <c r="D35" s="75"/>
+      <c r="E35" s="81"/>
+      <c r="F35" s="82"/>
+      <c r="G35" s="77">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="H35" s="47"/>
+      <c r="I35" s="16"/>
+      <c r="J35" s="25"/>
+      <c r="K35" s="13"/>
+      <c r="L35" s="14"/>
+      <c r="M35" s="64"/>
+      <c r="N35" s="15"/>
+      <c r="O35" s="16"/>
+      <c r="P35" s="60"/>
+      <c r="Q35" s="3" t="e">
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="S30" s="72"/>
-      <c r="T30" s="3">
+      <c r="S35" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A31" s="31">
-        <v>44915</v>
-      </c>
-      <c r="B31" s="3">
-        <v>30</v>
-      </c>
-      <c r="C31" s="81" t="s">
-        <v>54</v>
-      </c>
-      <c r="D31" s="82"/>
-      <c r="E31" s="12">
-        <v>55</v>
-      </c>
-      <c r="F31" s="13">
-        <v>41</v>
-      </c>
-      <c r="G31" s="14">
-        <v>14</v>
-      </c>
-      <c r="H31" s="32">
-        <v>10</v>
-      </c>
-      <c r="I31" s="19">
-        <v>61</v>
-      </c>
-      <c r="J31" s="28">
-        <v>-3.67</v>
-      </c>
-      <c r="K31" s="33"/>
-      <c r="L31" s="16">
-        <v>59.33</v>
-      </c>
-      <c r="M31" s="17"/>
-      <c r="N31" s="75">
-        <v>81</v>
-      </c>
-      <c r="O31" s="18"/>
-      <c r="P31" s="19">
-        <v>30</v>
-      </c>
-      <c r="Q31" s="71">
-        <v>113</v>
-      </c>
-      <c r="R31" s="3">
-        <f t="shared" si="2"/>
-        <v>74.336283185840713</v>
-      </c>
-      <c r="S31" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="T31" s="3">
-        <f t="shared" si="1"/>
-        <v>21.67</v>
-      </c>
-    </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A32" s="31">
-        <v>44917</v>
-      </c>
-      <c r="B32" s="3">
+    <row r="36" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="28"/>
+      <c r="B36" s="3">
         <v>31</v>
       </c>
-      <c r="C32" s="81" t="s">
-        <v>55</v>
-      </c>
-      <c r="D32" s="82"/>
-      <c r="E32" s="12">
-        <v>52</v>
-      </c>
-      <c r="F32" s="13">
-        <v>37</v>
-      </c>
-      <c r="G32" s="14">
-        <v>15</v>
-      </c>
-      <c r="H32" s="32">
-        <v>13</v>
-      </c>
-      <c r="I32" s="19">
-        <v>55</v>
-      </c>
-      <c r="J32" s="28">
-        <v>-3</v>
-      </c>
-      <c r="K32" s="33"/>
-      <c r="L32" s="16">
-        <v>52</v>
-      </c>
-      <c r="M32" s="17"/>
-      <c r="N32" s="75">
-        <v>81</v>
-      </c>
-      <c r="O32" s="18"/>
-      <c r="P32" s="19"/>
-      <c r="Q32" s="71"/>
-      <c r="R32" s="3" t="e">
-        <f t="shared" si="2"/>
+      <c r="C36" s="75" t="s">
+        <v>48</v>
+      </c>
+      <c r="D36" s="75"/>
+      <c r="E36" s="81"/>
+      <c r="F36" s="82"/>
+      <c r="G36" s="77">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="H36" s="47"/>
+      <c r="I36" s="16"/>
+      <c r="J36" s="25"/>
+      <c r="K36" s="13"/>
+      <c r="L36" s="14"/>
+      <c r="M36" s="64"/>
+      <c r="N36" s="15"/>
+      <c r="O36" s="16"/>
+      <c r="P36" s="60"/>
+      <c r="Q36" s="3" t="e">
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="S32" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="T32" s="3">
-        <f t="shared" si="1"/>
-        <v>29</v>
-      </c>
-    </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A33" s="31">
-        <v>44925</v>
-      </c>
-      <c r="B33" s="3">
-        <v>32</v>
-      </c>
-      <c r="C33" s="81" t="s">
-        <v>56</v>
-      </c>
-      <c r="D33" s="82"/>
-      <c r="E33" s="12">
-        <v>58</v>
-      </c>
-      <c r="F33" s="13">
-        <v>48</v>
-      </c>
-      <c r="G33" s="14">
-        <v>10</v>
-      </c>
-      <c r="H33" s="32">
-        <v>7</v>
-      </c>
-      <c r="I33" s="19">
-        <v>71</v>
-      </c>
-      <c r="J33" s="28">
-        <v>-1</v>
-      </c>
-      <c r="K33" s="33">
-        <v>28</v>
-      </c>
-      <c r="L33" s="16">
-        <v>70</v>
-      </c>
-      <c r="M33" s="17">
-        <v>44.97</v>
-      </c>
-      <c r="N33" s="75">
-        <v>79</v>
-      </c>
-      <c r="O33" s="18"/>
-      <c r="P33" s="19">
-        <v>6</v>
-      </c>
-      <c r="Q33" s="71">
-        <v>68</v>
-      </c>
-      <c r="R33" s="3">
-        <f t="shared" si="2"/>
-        <v>92.64705882352942</v>
-      </c>
-      <c r="S33" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="T33" s="3">
-        <f t="shared" si="1"/>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A34" s="31"/>
-      <c r="B34" s="3"/>
-      <c r="C34" s="81"/>
-      <c r="D34" s="82"/>
-      <c r="E34" s="12"/>
-      <c r="F34" s="13"/>
-      <c r="G34" s="14"/>
-      <c r="H34" s="32"/>
-      <c r="I34" s="19"/>
-      <c r="J34" s="28"/>
-      <c r="K34" s="33"/>
-      <c r="L34" s="16"/>
-      <c r="M34" s="17"/>
-      <c r="N34" s="75"/>
-      <c r="O34" s="18"/>
-      <c r="P34" s="19"/>
-      <c r="Q34" s="71"/>
-      <c r="R34" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S34" s="1"/>
-      <c r="T34" s="3">
+      <c r="S36" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A35" s="31"/>
-      <c r="B35" s="3">
-        <v>30</v>
-      </c>
-      <c r="C35" s="83" t="s">
-        <v>48</v>
-      </c>
-      <c r="D35" s="83"/>
-      <c r="E35" s="12"/>
-      <c r="F35" s="13"/>
-      <c r="G35" s="14"/>
-      <c r="H35" s="32"/>
-      <c r="I35" s="19"/>
-      <c r="J35" s="28"/>
-      <c r="K35" s="33"/>
-      <c r="L35" s="16"/>
-      <c r="M35" s="17"/>
-      <c r="N35" s="75"/>
-      <c r="O35" s="18"/>
-      <c r="P35" s="19"/>
-      <c r="Q35" s="71"/>
-      <c r="R35" s="3" t="e">
-        <f t="shared" si="2"/>
+    <row r="37" spans="1:19" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="28"/>
+      <c r="B37" s="3">
+        <v>32</v>
+      </c>
+      <c r="C37" s="75" t="s">
+        <v>49</v>
+      </c>
+      <c r="D37" s="75"/>
+      <c r="E37" s="81"/>
+      <c r="F37" s="82"/>
+      <c r="G37" s="77">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="H37" s="47"/>
+      <c r="I37" s="16"/>
+      <c r="J37" s="25"/>
+      <c r="K37" s="13"/>
+      <c r="L37" s="14"/>
+      <c r="M37" s="64"/>
+      <c r="N37" s="15"/>
+      <c r="O37" s="16"/>
+      <c r="P37" s="60"/>
+      <c r="Q37" s="3" t="e">
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="T35" s="3">
+      <c r="S37" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A36" s="31"/>
-      <c r="B36" s="3">
-        <v>31</v>
-      </c>
-      <c r="C36" s="83" t="s">
-        <v>49</v>
-      </c>
-      <c r="D36" s="83"/>
-      <c r="E36" s="12"/>
-      <c r="F36" s="13"/>
-      <c r="G36" s="14"/>
-      <c r="H36" s="32"/>
-      <c r="I36" s="19"/>
-      <c r="J36" s="28"/>
-      <c r="K36" s="33"/>
-      <c r="L36" s="16"/>
-      <c r="M36" s="17"/>
-      <c r="N36" s="75"/>
-      <c r="O36" s="18"/>
-      <c r="P36" s="19"/>
-      <c r="Q36" s="71"/>
-      <c r="R36" s="3" t="e">
-        <f t="shared" si="2"/>
+    <row r="38" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A38" s="28"/>
+      <c r="B38" s="3">
+        <v>33</v>
+      </c>
+      <c r="C38" s="75" t="s">
+        <v>50</v>
+      </c>
+      <c r="D38" s="75"/>
+      <c r="E38" s="81"/>
+      <c r="F38" s="82"/>
+      <c r="G38" s="77">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="H38" s="47"/>
+      <c r="I38" s="16"/>
+      <c r="J38" s="25"/>
+      <c r="K38" s="13"/>
+      <c r="L38" s="14"/>
+      <c r="M38" s="64"/>
+      <c r="N38" s="15"/>
+      <c r="O38" s="16"/>
+      <c r="P38" s="60"/>
+      <c r="Q38" s="3" t="e">
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="T36" s="3">
+      <c r="S38" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="31"/>
-      <c r="B37" s="3">
-        <v>32</v>
-      </c>
-      <c r="C37" s="83" t="s">
-        <v>50</v>
-      </c>
-      <c r="D37" s="83"/>
-      <c r="E37" s="12"/>
-      <c r="F37" s="13"/>
-      <c r="G37" s="14"/>
-      <c r="H37" s="32"/>
-      <c r="I37" s="19"/>
-      <c r="J37" s="28"/>
-      <c r="K37" s="33"/>
-      <c r="L37" s="16"/>
-      <c r="M37" s="17"/>
-      <c r="N37" s="75"/>
-      <c r="O37" s="18"/>
-      <c r="P37" s="19"/>
-      <c r="Q37" s="71"/>
-      <c r="R37" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T37" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A38" s="31"/>
-      <c r="B38" s="3">
-        <v>33</v>
-      </c>
-      <c r="C38" s="83" t="s">
-        <v>51</v>
-      </c>
-      <c r="D38" s="83"/>
-      <c r="E38" s="12"/>
-      <c r="F38" s="13"/>
-      <c r="G38" s="14"/>
-      <c r="H38" s="32"/>
-      <c r="I38" s="19"/>
-      <c r="J38" s="28"/>
-      <c r="K38" s="33"/>
-      <c r="L38" s="16"/>
-      <c r="M38" s="17"/>
-      <c r="N38" s="75"/>
-      <c r="O38" s="18"/>
-      <c r="P38" s="19"/>
-      <c r="Q38" s="71"/>
-      <c r="R38" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T38" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A39" s="3"/>
       <c r="B39" s="3">
         <v>34</v>
       </c>
-      <c r="C39" s="84" t="s">
-        <v>21</v>
-      </c>
-      <c r="D39" s="84"/>
-      <c r="E39" s="12">
-        <f t="shared" ref="E39:P39" si="3">AVERAGE(E2:E38)</f>
-        <v>55.4</v>
-      </c>
-      <c r="F39" s="13">
-        <f t="shared" si="3"/>
-        <v>41.551724137931032</v>
-      </c>
-      <c r="G39" s="14">
-        <f t="shared" si="3"/>
-        <v>14.033333333333333</v>
-      </c>
-      <c r="H39" s="15">
-        <f t="shared" si="3"/>
-        <v>9.6</v>
-      </c>
-      <c r="I39" s="19">
-        <f t="shared" si="3"/>
-        <v>61.8</v>
-      </c>
-      <c r="J39" s="28">
-        <f t="shared" si="3"/>
-        <v>-2.8770000000000002</v>
-      </c>
-      <c r="K39" s="15">
-        <f t="shared" si="3"/>
-        <v>16.125</v>
-      </c>
-      <c r="L39" s="16">
-        <f t="shared" si="3"/>
-        <v>59.05599999999999</v>
-      </c>
-      <c r="M39" s="17">
-        <f t="shared" si="3"/>
-        <v>41.157407407407419</v>
-      </c>
-      <c r="N39" s="75">
-        <f t="shared" si="3"/>
-        <v>82.057333333333332</v>
-      </c>
-      <c r="O39" s="18">
-        <f t="shared" si="3"/>
-        <v>73.213043478260872</v>
-      </c>
-      <c r="P39" s="19">
-        <f t="shared" si="3"/>
-        <v>117.32142857142857</v>
-      </c>
-      <c r="Q39" s="71"/>
-      <c r="R39" s="3" t="e">
-        <f t="shared" si="2"/>
+      <c r="C39" s="71" t="s">
+        <v>20</v>
+      </c>
+      <c r="D39" s="71"/>
+      <c r="E39" s="81">
+        <f t="shared" ref="E39:O39" si="6">AVERAGE(E2:E38)</f>
+        <v>55.6875</v>
+      </c>
+      <c r="F39" s="82">
+        <f t="shared" si="6"/>
+        <v>42.064516129032256</v>
+      </c>
+      <c r="G39" s="83">
+        <f t="shared" si="6"/>
+        <v>11.945945945945946</v>
+      </c>
+      <c r="H39" s="12">
+        <f t="shared" si="6"/>
+        <v>9.3125</v>
+      </c>
+      <c r="I39" s="16">
+        <f t="shared" si="6"/>
+        <v>62.625</v>
+      </c>
+      <c r="J39" s="25">
+        <f t="shared" si="6"/>
+        <v>-2.8421875000000001</v>
+      </c>
+      <c r="K39" s="13">
+        <f t="shared" si="6"/>
+        <v>59.907187499999992</v>
+      </c>
+      <c r="L39" s="14">
+        <f t="shared" si="6"/>
+        <v>41.300000000000004</v>
+      </c>
+      <c r="M39" s="64">
+        <f t="shared" si="6"/>
+        <v>81.845312499999991</v>
+      </c>
+      <c r="N39" s="15">
+        <f t="shared" si="6"/>
+        <v>73.535416666666677</v>
+      </c>
+      <c r="O39" s="16">
+        <f t="shared" si="6"/>
+        <v>109.8</v>
+      </c>
+      <c r="P39" s="60"/>
+      <c r="Q39" s="3" t="e">
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="T39" s="3">
+      <c r="S39" s="3">
         <f t="shared" si="1"/>
-        <v>23.001333333333342</v>
+        <v>21.938124999999999</v>
       </c>
     </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B40" s="3"/>
-      <c r="E40" s="20"/>
-      <c r="F40" s="21"/>
-      <c r="G40" s="22"/>
-      <c r="H40" s="23"/>
-      <c r="I40" s="27"/>
-      <c r="J40" s="29"/>
-      <c r="K40" s="23"/>
-      <c r="L40" s="24"/>
-      <c r="M40" s="25"/>
-      <c r="N40" s="78"/>
-      <c r="O40" s="26"/>
-      <c r="P40" s="27"/>
-      <c r="Q40" s="27"/>
+      <c r="E40" s="17"/>
+      <c r="F40" s="18"/>
+      <c r="G40" s="19"/>
+      <c r="H40" s="20"/>
+      <c r="I40" s="24"/>
+      <c r="J40" s="26"/>
+      <c r="K40" s="21"/>
+      <c r="L40" s="22"/>
+      <c r="M40" s="67"/>
+      <c r="N40" s="23"/>
+      <c r="O40" s="24"/>
+      <c r="P40" s="24"/>
     </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B41" s="3"/>
-      <c r="E41" s="20"/>
-      <c r="F41" s="21"/>
-      <c r="G41" s="22"/>
-      <c r="H41" s="23"/>
-      <c r="I41" s="27"/>
-      <c r="J41" s="29"/>
-      <c r="K41" s="23"/>
-      <c r="L41" s="24"/>
-      <c r="M41" s="25"/>
-      <c r="N41" s="78"/>
-      <c r="O41" s="26"/>
-      <c r="P41" s="27"/>
-      <c r="Q41" s="27"/>
+      <c r="E41" s="17"/>
+      <c r="F41" s="18"/>
+      <c r="G41" s="19"/>
+      <c r="H41" s="20"/>
+      <c r="I41" s="24"/>
+      <c r="J41" s="26"/>
+      <c r="K41" s="21"/>
+      <c r="L41" s="22"/>
+      <c r="M41" s="67"/>
+      <c r="N41" s="23"/>
+      <c r="O41" s="24"/>
+      <c r="P41" s="24"/>
     </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="E42" s="20"/>
-      <c r="F42" s="21"/>
-      <c r="G42" s="22"/>
-      <c r="H42" s="23"/>
-      <c r="I42" s="27"/>
-      <c r="J42" s="29"/>
-      <c r="K42" s="23"/>
-      <c r="L42" s="24"/>
-      <c r="M42" s="25"/>
-      <c r="N42" s="78"/>
-      <c r="O42" s="26"/>
-      <c r="P42" s="27"/>
-      <c r="Q42" s="27"/>
+    <row r="42" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="E42" s="17"/>
+      <c r="F42" s="18"/>
+      <c r="G42" s="19"/>
+      <c r="H42" s="20"/>
+      <c r="I42" s="24"/>
+      <c r="J42" s="26"/>
+      <c r="K42" s="21"/>
+      <c r="L42" s="22"/>
+      <c r="M42" s="67"/>
+      <c r="N42" s="23"/>
+      <c r="O42" s="24"/>
+      <c r="P42" s="24"/>
     </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="E43" s="20"/>
-      <c r="F43" s="21"/>
-      <c r="G43" s="22"/>
-      <c r="H43" s="23"/>
-      <c r="I43" s="27"/>
-      <c r="J43" s="29"/>
-      <c r="K43" s="23"/>
-      <c r="L43" s="24"/>
-      <c r="M43" s="25"/>
-      <c r="N43" s="78"/>
-      <c r="O43" s="26"/>
-      <c r="P43" s="27"/>
-      <c r="Q43" s="27"/>
+    <row r="43" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="E43" s="17"/>
+      <c r="F43" s="18"/>
+      <c r="G43" s="19"/>
+      <c r="H43" s="20"/>
+      <c r="I43" s="24"/>
+      <c r="J43" s="26"/>
+      <c r="K43" s="21"/>
+      <c r="L43" s="22"/>
+      <c r="M43" s="67"/>
+      <c r="N43" s="23"/>
+      <c r="O43" s="24"/>
+      <c r="P43" s="24"/>
     </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="E44" s="20"/>
-      <c r="F44" s="21"/>
-      <c r="G44" s="22"/>
-      <c r="H44" s="23"/>
-      <c r="I44" s="27"/>
-      <c r="J44" s="29"/>
-      <c r="K44" s="23"/>
-      <c r="L44" s="24"/>
-      <c r="M44" s="25"/>
-      <c r="N44" s="78"/>
-      <c r="O44" s="26"/>
-      <c r="P44" s="27"/>
-      <c r="Q44" s="27"/>
+    <row r="44" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="E44" s="17"/>
+      <c r="F44" s="18"/>
+      <c r="G44" s="19"/>
+      <c r="H44" s="20"/>
+      <c r="I44" s="24"/>
+      <c r="J44" s="26"/>
+      <c r="K44" s="21"/>
+      <c r="L44" s="22"/>
+      <c r="M44" s="67"/>
+      <c r="N44" s="23"/>
+      <c r="O44" s="24"/>
+      <c r="P44" s="24"/>
     </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="E45" s="20"/>
-      <c r="F45" s="21"/>
-      <c r="G45" s="22"/>
-      <c r="H45" s="23"/>
-      <c r="I45" s="27"/>
-      <c r="J45" s="29"/>
-      <c r="K45" s="23"/>
-      <c r="L45" s="24"/>
-      <c r="M45" s="25"/>
-      <c r="N45" s="78"/>
-      <c r="O45" s="26"/>
-      <c r="P45" s="27"/>
-      <c r="Q45" s="27"/>
+    <row r="45" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="E45" s="17"/>
+      <c r="F45" s="18"/>
+      <c r="G45" s="19"/>
+      <c r="H45" s="20"/>
+      <c r="I45" s="24"/>
+      <c r="J45" s="26"/>
+      <c r="K45" s="21"/>
+      <c r="L45" s="22"/>
+      <c r="M45" s="67"/>
+      <c r="N45" s="23"/>
+      <c r="O45" s="24"/>
+      <c r="P45" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="39">
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C29:D29"/>
     <mergeCell ref="C39:D39"/>
     <mergeCell ref="C11:D11"/>
     <mergeCell ref="C1:D1"/>
@@ -7392,23 +7578,19 @@
     <mergeCell ref="C20:D20"/>
     <mergeCell ref="C21:D21"/>
     <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C15:D15"/>
   </mergeCells>
-  <conditionalFormatting sqref="M2:M14">
-    <cfRule type="colorScale" priority="90">
+  <phoneticPr fontId="3" type="noConversion"/>
+  <conditionalFormatting sqref="L2:L14">
+    <cfRule type="colorScale" priority="91">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -7419,7 +7601,19 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M22:M24 M26 M29:M34">
+  <conditionalFormatting sqref="L22:L24 L26 L29:L34">
+    <cfRule type="colorScale" priority="88">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K22:K24 K26 K29:K34">
     <cfRule type="colorScale" priority="87">
       <colorScale>
         <cfvo type="min"/>
@@ -7431,20 +7625,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L22:L24 L26 L29:L34">
-    <cfRule type="colorScale" priority="86">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O22:O24 O26 O29:O34">
-    <cfRule type="iconSet" priority="85">
+  <conditionalFormatting sqref="N22:N24 N26 N29:N34">
+    <cfRule type="iconSet" priority="86">
       <iconSet iconSet="3Arrows">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="33"/>
@@ -7453,7 +7635,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I22:I24 I26 I29:I34">
-    <cfRule type="dataBar" priority="84">
+    <cfRule type="dataBar" priority="85">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -7467,7 +7649,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J22:J24 J26 J29:J34">
-    <cfRule type="iconSet" priority="91">
+    <cfRule type="iconSet" priority="92">
       <iconSet iconSet="3Arrows">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="33"/>
@@ -7476,7 +7658,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F22:F24 F26 F29:F34">
-    <cfRule type="colorScale" priority="92">
+    <cfRule type="colorScale" priority="93">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -7486,28 +7668,28 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="92" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="11" priority="93" operator="greaterThan">
       <formula>$G$24</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P22:P24 P26 P29:P34">
-    <cfRule type="cellIs" dxfId="14" priority="71" operator="between">
+  <conditionalFormatting sqref="O22:O24 O26 O29:O34">
+    <cfRule type="cellIs" dxfId="10" priority="72" operator="between">
       <formula>1</formula>
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S22:S34">
-    <cfRule type="cellIs" dxfId="13" priority="70" operator="equal">
+  <conditionalFormatting sqref="R2:R34">
+    <cfRule type="cellIs" dxfId="9" priority="71" operator="equal">
       <formula>"NO"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S22:S34">
-    <cfRule type="cellIs" dxfId="12" priority="69" operator="equal">
+  <conditionalFormatting sqref="R2:R34">
+    <cfRule type="cellIs" dxfId="8" priority="70" operator="equal">
       <formula>"YES"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L2:L21">
-    <cfRule type="colorScale" priority="97">
+  <conditionalFormatting sqref="K2:K21">
+    <cfRule type="colorScale" priority="98">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -7518,8 +7700,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O2:O21">
-    <cfRule type="iconSet" priority="98">
+  <conditionalFormatting sqref="N2:N21">
+    <cfRule type="iconSet" priority="99">
       <iconSet iconSet="3Arrows">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="33"/>
@@ -7528,7 +7710,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I21">
-    <cfRule type="dataBar" priority="99">
+    <cfRule type="dataBar" priority="100">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -7542,7 +7724,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:J21">
-    <cfRule type="iconSet" priority="100">
+    <cfRule type="iconSet" priority="101">
       <iconSet iconSet="3Arrows">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="33"/>
@@ -7550,8 +7732,8 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M2:M21">
-    <cfRule type="colorScale" priority="104">
+  <conditionalFormatting sqref="L2:L21">
+    <cfRule type="colorScale" priority="105">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -7562,7 +7744,19 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M25">
+  <conditionalFormatting sqref="L25">
+    <cfRule type="colorScale" priority="53">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K25">
     <cfRule type="colorScale" priority="52">
       <colorScale>
         <cfvo type="min"/>
@@ -7574,20 +7768,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L25">
-    <cfRule type="colorScale" priority="51">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O25">
-    <cfRule type="iconSet" priority="50">
+  <conditionalFormatting sqref="N25">
+    <cfRule type="iconSet" priority="51">
       <iconSet iconSet="3Arrows">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="33"/>
@@ -7596,7 +7778,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I25">
-    <cfRule type="dataBar" priority="49">
+    <cfRule type="dataBar" priority="50">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -7610,7 +7792,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J25">
-    <cfRule type="iconSet" priority="105">
+    <cfRule type="iconSet" priority="106">
       <iconSet iconSet="3Arrows">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="33"/>
@@ -7619,7 +7801,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F25">
-    <cfRule type="colorScale" priority="106">
+    <cfRule type="colorScale" priority="107">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -7629,18 +7811,18 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="106" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="7" priority="107" operator="greaterThan">
       <formula>$G$24</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P25">
-    <cfRule type="cellIs" dxfId="10" priority="44" operator="between">
+  <conditionalFormatting sqref="O25">
+    <cfRule type="cellIs" dxfId="6" priority="45" operator="between">
       <formula>1</formula>
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R1:R1048576">
-    <cfRule type="colorScale" priority="40">
+  <conditionalFormatting sqref="Q1:Q1048576">
+    <cfRule type="colorScale" priority="41">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -7651,8 +7833,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N1:N26 N29:N1048576">
-    <cfRule type="colorScale" priority="39">
+  <conditionalFormatting sqref="M1:M26 M29:M1048576">
+    <cfRule type="colorScale" priority="40">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -7663,7 +7845,19 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M27">
+  <conditionalFormatting sqref="L27">
+    <cfRule type="colorScale" priority="39">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K27">
     <cfRule type="colorScale" priority="38">
       <colorScale>
         <cfvo type="min"/>
@@ -7675,20 +7869,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L27">
-    <cfRule type="colorScale" priority="37">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O27">
-    <cfRule type="iconSet" priority="36">
+  <conditionalFormatting sqref="N27">
+    <cfRule type="iconSet" priority="37">
       <iconSet iconSet="3Arrows">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="33"/>
@@ -7697,7 +7879,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I27">
-    <cfRule type="dataBar" priority="35">
+    <cfRule type="dataBar" priority="36">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -7711,7 +7893,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J27">
-    <cfRule type="iconSet" priority="107">
+    <cfRule type="iconSet" priority="108">
       <iconSet iconSet="3Arrows">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="33"/>
@@ -7720,21 +7902,6 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F27">
-    <cfRule type="colorScale" priority="108">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="108" operator="greaterThan">
-      <formula>$G$24</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N27">
     <cfRule type="colorScale" priority="109">
       <colorScale>
         <cfvo type="min"/>
@@ -7745,15 +7912,12 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P27">
-    <cfRule type="cellIs" dxfId="8" priority="22" operator="between">
-      <formula>1</formula>
-      <formula>10</formula>
+    <cfRule type="cellIs" dxfId="5" priority="109" operator="greaterThan">
+      <formula>$G$24</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M28">
-    <cfRule type="colorScale" priority="12">
+  <conditionalFormatting sqref="M27">
+    <cfRule type="colorScale" priority="110">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -7762,6 +7926,12 @@
         <color rgb="FFFCFCFF"/>
         <color rgb="FF63BE7B"/>
       </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O27">
+    <cfRule type="cellIs" dxfId="4" priority="23" operator="between">
+      <formula>1</formula>
+      <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L28">
@@ -7776,8 +7946,20 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O28">
-    <cfRule type="iconSet" priority="14">
+  <conditionalFormatting sqref="K28">
+    <cfRule type="colorScale" priority="14">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N28">
+    <cfRule type="iconSet" priority="15">
       <iconSet iconSet="3Arrows">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="33"/>
@@ -7786,7 +7968,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I28">
-    <cfRule type="dataBar" priority="15">
+    <cfRule type="dataBar" priority="16">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -7800,7 +7982,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J28">
-    <cfRule type="iconSet" priority="16">
+    <cfRule type="iconSet" priority="17">
       <iconSet iconSet="3Arrows">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="33"/>
@@ -7809,7 +7991,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F28">
-    <cfRule type="colorScale" priority="17">
+    <cfRule type="colorScale" priority="18">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -7819,12 +8001,12 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="18" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="19" operator="greaterThan">
       <formula>$G$24</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N28">
-    <cfRule type="colorScale" priority="19">
+  <conditionalFormatting sqref="M28">
+    <cfRule type="colorScale" priority="20">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -7835,14 +8017,14 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P28">
-    <cfRule type="cellIs" dxfId="4" priority="3" operator="between">
+  <conditionalFormatting sqref="O28">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="between">
       <formula>1</formula>
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L35:L38">
-    <cfRule type="colorScale" priority="110">
+  <conditionalFormatting sqref="K35:K38">
+    <cfRule type="colorScale" priority="111">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -7853,8 +8035,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O35:O38">
-    <cfRule type="iconSet" priority="112">
+  <conditionalFormatting sqref="N35:N38">
+    <cfRule type="iconSet" priority="113">
       <iconSet iconSet="3Arrows">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="33"/>
@@ -7863,7 +8045,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I35:I38">
-    <cfRule type="dataBar" priority="114">
+    <cfRule type="dataBar" priority="115">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -7877,7 +8059,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J35:J38">
-    <cfRule type="iconSet" priority="116">
+    <cfRule type="iconSet" priority="117">
       <iconSet iconSet="3Arrows">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="33"/>
@@ -7886,7 +8068,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F35:F38">
-    <cfRule type="colorScale" priority="118">
+    <cfRule type="colorScale" priority="119">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -7896,12 +8078,12 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="119" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="120" operator="greaterThan">
       <formula>$G$24</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M35:M38">
-    <cfRule type="colorScale" priority="122">
+  <conditionalFormatting sqref="L35:L38">
+    <cfRule type="colorScale" priority="123">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -7913,7 +8095,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F21">
-    <cfRule type="colorScale" priority="124">
+    <cfRule type="colorScale" priority="125">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -7923,12 +8105,12 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="125" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="126" operator="greaterThan">
       <formula>$F$39</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T2:T39">
-    <cfRule type="colorScale" priority="126">
+  <conditionalFormatting sqref="S2:S39">
+    <cfRule type="colorScale" priority="127">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -7936,6 +8118,18 @@
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F2:F38">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Added marks of Made Easy GATE Mock 1
</commit_message>
<xml_diff>
--- a/My Marks Tracker.xlsx
+++ b/My Marks Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GATE 2022 &amp; 2023\My Progress trackers &amp; Journey - In Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9C439B7-7061-4BB3-B86C-4F7CBC503A90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7477E371-A80B-4684-BED1-3669729BC752}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3209D17C-0F5C-4895-BA2D-FBE4C1879A87}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="61">
   <si>
     <t>Test Name</t>
   </si>
@@ -728,13 +728,29 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -746,23 +762,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -794,17 +794,21 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="4" tint="-0.24994659260841701"/>
+          <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
         </patternFill>
       </fill>
     </dxf>
@@ -826,9 +830,12 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
       <fill>
         <patternFill>
-          <bgColor theme="4" tint="-0.24994659260841701"/>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -856,13 +863,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="-0.24994659260841701"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1181,6 +1181,9 @@
                 </c:pt>
                 <c:pt idx="34">
                   <c:v>52.33</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>64.03</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1616,6 +1619,9 @@
                 <c:pt idx="28">
                   <c:v>80.95</c:v>
                 </c:pt>
+                <c:pt idx="35">
+                  <c:v>70.97</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1983,7 +1989,7 @@
                   <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0</c:v>
+                  <c:v>6.3299999999999983</c:v>
                 </c:pt>
                 <c:pt idx="36">
                   <c:v>0</c:v>
@@ -2369,7 +2375,7 @@
                   <c:v>84.033613445378151</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0</c:v>
+                  <c:v>93.45794392523365</c:v>
                 </c:pt>
                 <c:pt idx="36">
                   <c:v>0</c:v>
@@ -2382,6 +2388,9 @@
                 </c:pt>
                 <c:pt idx="39">
                   <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>54.17962902438336</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4732,16 +4741,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>541020</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>487231</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>68580</xdr:rowOff>
+      <xdr:rowOff>68579</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>441960</xdr:colOff>
-      <xdr:row>60</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>89647</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>134470</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4768,16 +4777,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>230393</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>144556</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>33170</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>63873</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>542813</xdr:colOff>
-      <xdr:row>61</xdr:row>
-      <xdr:rowOff>144556</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>309731</xdr:colOff>
+      <xdr:row>80</xdr:row>
+      <xdr:rowOff>63874</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5176,8 +5185,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E08F6CAB-EED7-4179-B275-45A8F5F85EF1}">
   <dimension ref="A1:S47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="S36" sqref="S36"/>
+    <sheetView tabSelected="1" topLeftCell="B19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q40" sqref="Q40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5209,10 +5218,10 @@
       <c r="B1" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="85" t="s">
+      <c r="C1" s="83" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="85"/>
+      <c r="D1" s="83"/>
       <c r="E1" s="30" t="s">
         <v>3</v>
       </c>
@@ -5264,10 +5273,10 @@
       <c r="B2" s="46">
         <v>1</v>
       </c>
-      <c r="C2" s="86" t="s">
+      <c r="C2" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="86"/>
+      <c r="D2" s="84"/>
       <c r="E2" s="47">
         <v>41</v>
       </c>
@@ -5323,10 +5332,10 @@
       <c r="B3" s="49">
         <v>2</v>
       </c>
-      <c r="C3" s="84" t="s">
+      <c r="C3" s="81" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="84"/>
+      <c r="D3" s="81"/>
       <c r="E3" s="50">
         <v>40</v>
       </c>
@@ -5382,10 +5391,10 @@
       <c r="B4" s="49">
         <v>3</v>
       </c>
-      <c r="C4" s="84" t="s">
+      <c r="C4" s="81" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="84"/>
+      <c r="D4" s="81"/>
       <c r="E4" s="50">
         <v>51</v>
       </c>
@@ -5397,7 +5406,7 @@
         <v>18</v>
       </c>
       <c r="H4" s="47">
-        <f t="shared" ref="H4:H36" si="3">65-E4</f>
+        <f t="shared" ref="H4:H37" si="3">65-E4</f>
         <v>14</v>
       </c>
       <c r="I4" s="50">
@@ -5441,10 +5450,10 @@
       <c r="B5" s="49">
         <v>4</v>
       </c>
-      <c r="C5" s="84" t="s">
+      <c r="C5" s="81" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="84"/>
+      <c r="D5" s="81"/>
       <c r="E5" s="50">
         <v>51</v>
       </c>
@@ -5491,10 +5500,10 @@
       <c r="B6" s="49">
         <v>5</v>
       </c>
-      <c r="C6" s="84" t="s">
+      <c r="C6" s="81" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="84"/>
+      <c r="D6" s="81"/>
       <c r="E6" s="50">
         <v>47</v>
       </c>
@@ -5550,10 +5559,10 @@
       <c r="B7" s="49">
         <v>6</v>
       </c>
-      <c r="C7" s="84" t="s">
+      <c r="C7" s="81" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="84"/>
+      <c r="D7" s="81"/>
       <c r="E7" s="50">
         <v>51</v>
       </c>
@@ -5609,10 +5618,10 @@
       <c r="B8" s="49">
         <v>7</v>
       </c>
-      <c r="C8" s="84" t="s">
+      <c r="C8" s="81" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="84"/>
+      <c r="D8" s="81"/>
       <c r="E8" s="50">
         <v>52</v>
       </c>
@@ -5668,10 +5677,10 @@
       <c r="B9" s="49">
         <v>8</v>
       </c>
-      <c r="C9" s="84" t="s">
+      <c r="C9" s="81" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="84"/>
+      <c r="D9" s="81"/>
       <c r="E9" s="50">
         <v>55</v>
       </c>
@@ -5727,10 +5736,10 @@
       <c r="B10" s="49">
         <v>9</v>
       </c>
-      <c r="C10" s="84" t="s">
+      <c r="C10" s="81" t="s">
         <v>25</v>
       </c>
-      <c r="D10" s="84"/>
+      <c r="D10" s="81"/>
       <c r="E10" s="50">
         <v>58</v>
       </c>
@@ -5786,10 +5795,10 @@
       <c r="B11" s="49">
         <v>10</v>
       </c>
-      <c r="C11" s="84" t="s">
+      <c r="C11" s="81" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="84"/>
+      <c r="D11" s="81"/>
       <c r="E11" s="50">
         <v>60</v>
       </c>
@@ -5845,10 +5854,10 @@
       <c r="B12" s="49">
         <v>11</v>
       </c>
-      <c r="C12" s="84" t="s">
+      <c r="C12" s="81" t="s">
         <v>27</v>
       </c>
-      <c r="D12" s="84"/>
+      <c r="D12" s="81"/>
       <c r="E12" s="50">
         <v>56</v>
       </c>
@@ -5904,10 +5913,10 @@
       <c r="B13" s="49">
         <v>12</v>
       </c>
-      <c r="C13" s="84" t="s">
+      <c r="C13" s="81" t="s">
         <v>28</v>
       </c>
-      <c r="D13" s="84"/>
+      <c r="D13" s="81"/>
       <c r="E13" s="50">
         <v>56</v>
       </c>
@@ -5963,10 +5972,10 @@
       <c r="B14" s="49">
         <v>13</v>
       </c>
-      <c r="C14" s="84" t="s">
+      <c r="C14" s="81" t="s">
         <v>29</v>
       </c>
-      <c r="D14" s="84"/>
+      <c r="D14" s="81"/>
       <c r="E14" s="50">
         <v>56</v>
       </c>
@@ -6022,10 +6031,10 @@
       <c r="B15" s="49">
         <v>14</v>
       </c>
-      <c r="C15" s="84" t="s">
+      <c r="C15" s="81" t="s">
         <v>30</v>
       </c>
-      <c r="D15" s="84"/>
+      <c r="D15" s="81"/>
       <c r="E15" s="50">
         <v>50</v>
       </c>
@@ -6079,10 +6088,10 @@
       <c r="B16" s="49">
         <v>15</v>
       </c>
-      <c r="C16" s="84" t="s">
+      <c r="C16" s="81" t="s">
         <v>31</v>
       </c>
-      <c r="D16" s="84"/>
+      <c r="D16" s="81"/>
       <c r="E16" s="50">
         <v>56</v>
       </c>
@@ -6136,10 +6145,10 @@
       <c r="B17" s="49">
         <v>16</v>
       </c>
-      <c r="C17" s="84" t="s">
+      <c r="C17" s="81" t="s">
         <v>32</v>
       </c>
-      <c r="D17" s="84"/>
+      <c r="D17" s="81"/>
       <c r="E17" s="50">
         <v>53</v>
       </c>
@@ -6193,10 +6202,10 @@
       <c r="B18" s="49">
         <v>17</v>
       </c>
-      <c r="C18" s="84" t="s">
+      <c r="C18" s="81" t="s">
         <v>33</v>
       </c>
-      <c r="D18" s="84"/>
+      <c r="D18" s="81"/>
       <c r="E18" s="50">
         <v>58</v>
       </c>
@@ -6252,10 +6261,10 @@
       <c r="B19" s="49">
         <v>18</v>
       </c>
-      <c r="C19" s="84" t="s">
+      <c r="C19" s="81" t="s">
         <v>34</v>
       </c>
-      <c r="D19" s="84"/>
+      <c r="D19" s="81"/>
       <c r="E19" s="50">
         <v>60</v>
       </c>
@@ -6311,10 +6320,10 @@
       <c r="B20" s="49">
         <v>19</v>
       </c>
-      <c r="C20" s="84" t="s">
+      <c r="C20" s="81" t="s">
         <v>35</v>
       </c>
-      <c r="D20" s="84"/>
+      <c r="D20" s="81"/>
       <c r="E20" s="50">
         <v>59</v>
       </c>
@@ -6370,10 +6379,10 @@
       <c r="B21" s="52">
         <v>20</v>
       </c>
-      <c r="C21" s="87" t="s">
+      <c r="C21" s="85" t="s">
         <v>36</v>
       </c>
-      <c r="D21" s="87"/>
+      <c r="D21" s="85"/>
       <c r="E21" s="53">
         <v>56</v>
       </c>
@@ -6431,10 +6440,10 @@
       <c r="B22" s="75">
         <v>21</v>
       </c>
-      <c r="C22" s="88" t="s">
+      <c r="C22" s="77" t="s">
         <v>37</v>
       </c>
-      <c r="D22" s="89"/>
+      <c r="D22" s="78"/>
       <c r="E22" s="70">
         <v>57</v>
       </c>
@@ -6492,10 +6501,10 @@
       <c r="B23" s="76">
         <v>22</v>
       </c>
-      <c r="C23" s="77" t="s">
+      <c r="C23" s="79" t="s">
         <v>39</v>
       </c>
-      <c r="D23" s="78"/>
+      <c r="D23" s="80"/>
       <c r="E23" s="72">
         <v>58</v>
       </c>
@@ -6553,10 +6562,10 @@
       <c r="B24" s="76">
         <v>23</v>
       </c>
-      <c r="C24" s="77" t="s">
+      <c r="C24" s="79" t="s">
         <v>40</v>
       </c>
-      <c r="D24" s="78"/>
+      <c r="D24" s="80"/>
       <c r="E24" s="72">
         <v>64</v>
       </c>
@@ -6614,10 +6623,10 @@
       <c r="B25" s="76">
         <v>24</v>
       </c>
-      <c r="C25" s="77" t="s">
+      <c r="C25" s="79" t="s">
         <v>41</v>
       </c>
-      <c r="D25" s="78"/>
+      <c r="D25" s="80"/>
       <c r="E25" s="72">
         <v>63</v>
       </c>
@@ -6675,10 +6684,10 @@
       <c r="B26" s="76">
         <v>25</v>
       </c>
-      <c r="C26" s="77" t="s">
+      <c r="C26" s="79" t="s">
         <v>42</v>
       </c>
-      <c r="D26" s="78"/>
+      <c r="D26" s="80"/>
       <c r="E26" s="72">
         <v>63</v>
       </c>
@@ -6736,10 +6745,10 @@
       <c r="B27" s="76">
         <v>26</v>
       </c>
-      <c r="C27" s="77" t="s">
+      <c r="C27" s="79" t="s">
         <v>43</v>
       </c>
-      <c r="D27" s="78"/>
+      <c r="D27" s="80"/>
       <c r="E27" s="72">
         <v>61</v>
       </c>
@@ -6797,10 +6806,10 @@
       <c r="B28" s="76">
         <v>27</v>
       </c>
-      <c r="C28" s="80" t="s">
+      <c r="C28" s="86" t="s">
         <v>44</v>
       </c>
-      <c r="D28" s="80"/>
+      <c r="D28" s="86"/>
       <c r="E28" s="72">
         <v>65</v>
       </c>
@@ -6856,10 +6865,10 @@
       <c r="B29" s="3">
         <v>28</v>
       </c>
-      <c r="C29" s="81" t="s">
+      <c r="C29" s="87" t="s">
         <v>45</v>
       </c>
-      <c r="D29" s="82"/>
+      <c r="D29" s="88"/>
       <c r="E29" s="72"/>
       <c r="F29" s="73"/>
       <c r="G29" s="50">
@@ -6892,10 +6901,10 @@
       <c r="B30" s="76">
         <v>29</v>
       </c>
-      <c r="C30" s="77" t="s">
+      <c r="C30" s="79" t="s">
         <v>46</v>
       </c>
-      <c r="D30" s="78"/>
+      <c r="D30" s="80"/>
       <c r="E30" s="72">
         <v>63</v>
       </c>
@@ -6953,10 +6962,10 @@
       <c r="B31" s="76">
         <v>30</v>
       </c>
-      <c r="C31" s="77" t="s">
+      <c r="C31" s="79" t="s">
         <v>53</v>
       </c>
-      <c r="D31" s="78"/>
+      <c r="D31" s="80"/>
       <c r="E31" s="72">
         <v>55</v>
       </c>
@@ -7010,10 +7019,10 @@
       <c r="B32" s="76">
         <v>31</v>
       </c>
-      <c r="C32" s="77" t="s">
+      <c r="C32" s="79" t="s">
         <v>54</v>
       </c>
-      <c r="D32" s="78"/>
+      <c r="D32" s="80"/>
       <c r="E32" s="72">
         <v>52</v>
       </c>
@@ -7063,10 +7072,10 @@
       <c r="B33" s="76">
         <v>32</v>
       </c>
-      <c r="C33" s="77" t="s">
+      <c r="C33" s="79" t="s">
         <v>55</v>
       </c>
-      <c r="D33" s="78"/>
+      <c r="D33" s="80"/>
       <c r="E33" s="72">
         <v>58</v>
       </c>
@@ -7122,10 +7131,10 @@
       <c r="B34" s="76">
         <v>33</v>
       </c>
-      <c r="C34" s="77" t="s">
+      <c r="C34" s="79" t="s">
         <v>56</v>
       </c>
-      <c r="D34" s="78"/>
+      <c r="D34" s="80"/>
       <c r="E34" s="72">
         <v>57</v>
       </c>
@@ -7181,10 +7190,10 @@
       <c r="B35" s="76">
         <v>34</v>
       </c>
-      <c r="C35" s="77" t="s">
+      <c r="C35" s="79" t="s">
         <v>59</v>
       </c>
-      <c r="D35" s="78"/>
+      <c r="D35" s="80"/>
       <c r="E35" s="72">
         <v>57</v>
       </c>
@@ -7239,10 +7248,10 @@
       <c r="B36" s="76">
         <v>35</v>
       </c>
-      <c r="C36" s="77" t="s">
+      <c r="C36" s="79" t="s">
         <v>60</v>
       </c>
-      <c r="D36" s="78"/>
+      <c r="D36" s="80"/>
       <c r="E36" s="72">
         <v>54</v>
       </c>
@@ -7291,36 +7300,64 @@
       </c>
     </row>
     <row r="37" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="28"/>
+      <c r="A37" s="28">
+        <v>44937</v>
+      </c>
       <c r="B37" s="76">
         <v>36</v>
       </c>
-      <c r="C37" s="79" t="s">
+      <c r="C37" s="86" t="s">
         <v>47</v>
       </c>
-      <c r="D37" s="79"/>
-      <c r="E37" s="72"/>
-      <c r="F37" s="73"/>
+      <c r="D37" s="86"/>
+      <c r="E37" s="72">
+        <v>62</v>
+      </c>
+      <c r="F37" s="73">
+        <v>44</v>
+      </c>
       <c r="G37" s="50">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="H37" s="47"/>
-      <c r="I37" s="16"/>
-      <c r="J37" s="25"/>
-      <c r="K37" s="13"/>
-      <c r="L37" s="14"/>
-      <c r="M37" s="64"/>
-      <c r="N37" s="15"/>
-      <c r="O37" s="16"/>
-      <c r="P37" s="60"/>
-      <c r="Q37" s="3" t="e">
+        <v>18</v>
+      </c>
+      <c r="H37" s="47">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="I37" s="16">
+        <v>67</v>
+      </c>
+      <c r="J37" s="25">
+        <v>-2.97</v>
+      </c>
+      <c r="K37" s="13">
+        <v>64.03</v>
+      </c>
+      <c r="L37" s="14">
+        <v>40.090000000000003</v>
+      </c>
+      <c r="M37" s="64">
+        <v>70.36</v>
+      </c>
+      <c r="N37" s="15">
+        <v>70.97</v>
+      </c>
+      <c r="O37" s="16">
+        <v>8</v>
+      </c>
+      <c r="P37" s="60">
+        <v>107</v>
+      </c>
+      <c r="Q37" s="3">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
+        <v>93.45794392523365</v>
+      </c>
+      <c r="R37" s="1" t="s">
+        <v>57</v>
       </c>
       <c r="S37" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>6.3299999999999983</v>
       </c>
     </row>
     <row r="38" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -7328,10 +7365,10 @@
       <c r="B38" s="76">
         <v>37</v>
       </c>
-      <c r="C38" s="79" t="s">
+      <c r="C38" s="89" t="s">
         <v>48</v>
       </c>
-      <c r="D38" s="79"/>
+      <c r="D38" s="89"/>
       <c r="E38" s="72"/>
       <c r="F38" s="73"/>
       <c r="G38" s="50">
@@ -7361,10 +7398,10 @@
       <c r="B39" s="76">
         <v>38</v>
       </c>
-      <c r="C39" s="79" t="s">
+      <c r="C39" s="89" t="s">
         <v>49</v>
       </c>
-      <c r="D39" s="79"/>
+      <c r="D39" s="89"/>
       <c r="E39" s="72"/>
       <c r="F39" s="73"/>
       <c r="G39" s="50">
@@ -7394,10 +7431,10 @@
       <c r="B40" s="76">
         <v>39</v>
       </c>
-      <c r="C40" s="79" t="s">
+      <c r="C40" s="89" t="s">
         <v>50</v>
       </c>
-      <c r="D40" s="79"/>
+      <c r="D40" s="89"/>
       <c r="E40" s="72"/>
       <c r="F40" s="73"/>
       <c r="G40" s="50">
@@ -7427,53 +7464,53 @@
       <c r="B41" s="76">
         <v>40</v>
       </c>
-      <c r="C41" s="83" t="s">
+      <c r="C41" s="82" t="s">
         <v>20</v>
       </c>
-      <c r="D41" s="83"/>
+      <c r="D41" s="82"/>
       <c r="E41" s="72">
         <f t="shared" ref="E41:O41" si="6">AVERAGE(E2:E40)</f>
-        <v>55.676470588235297</v>
+        <v>55.857142857142854</v>
       </c>
       <c r="F41" s="73">
         <f t="shared" si="6"/>
-        <v>41.666666666666664</v>
+        <v>41.735294117647058</v>
       </c>
       <c r="G41" s="74">
         <f t="shared" si="6"/>
-        <v>12.358974358974359</v>
+        <v>12.820512820512821</v>
       </c>
       <c r="H41" s="12">
         <f t="shared" si="6"/>
-        <v>9.3235294117647065</v>
+        <v>9.1428571428571423</v>
       </c>
       <c r="I41" s="16">
         <f t="shared" si="6"/>
-        <v>62</v>
+        <v>62.142857142857146</v>
       </c>
       <c r="J41" s="25">
         <f t="shared" si="6"/>
-        <v>-2.8908823529411767</v>
+        <v>-2.8931428571428572</v>
       </c>
       <c r="K41" s="13">
         <f t="shared" si="6"/>
-        <v>59.226176470588221</v>
+        <v>59.363428571428564</v>
       </c>
       <c r="L41" s="14">
         <f t="shared" si="6"/>
-        <v>40.842903225806452</v>
+        <v>40.819375000000001</v>
       </c>
       <c r="M41" s="64">
         <f t="shared" si="6"/>
-        <v>81.746470588235283</v>
+        <v>81.421142857142854</v>
       </c>
       <c r="N41" s="15">
         <f t="shared" si="6"/>
-        <v>73.535416666666677</v>
+        <v>73.4328</v>
       </c>
       <c r="O41" s="16">
         <f t="shared" si="6"/>
-        <v>106.96875</v>
+        <v>103.96969696969697</v>
       </c>
       <c r="P41" s="60"/>
       <c r="Q41" s="3" t="e">
@@ -7482,7 +7519,7 @@
       </c>
       <c r="S41" s="3">
         <f t="shared" si="1"/>
-        <v>22.520294117647062</v>
+        <v>22.05771428571429</v>
       </c>
     </row>
     <row r="42" spans="1:19" x14ac:dyDescent="0.3">
@@ -7499,6 +7536,10 @@
       <c r="N42" s="23"/>
       <c r="O42" s="24"/>
       <c r="P42" s="24"/>
+      <c r="Q42" s="3">
+        <f>AVERAGE(Q2:Q4)</f>
+        <v>54.17962902438336</v>
+      </c>
     </row>
     <row r="43" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B43" s="3"/>
@@ -7573,15 +7614,22 @@
     </row>
   </sheetData>
   <mergeCells count="41">
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C29:D29"/>
     <mergeCell ref="C41:D41"/>
     <mergeCell ref="C11:D11"/>
     <mergeCell ref="C1:D1"/>
@@ -7598,22 +7646,15 @@
     <mergeCell ref="C20:D20"/>
     <mergeCell ref="C21:D21"/>
     <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C15:D15"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="L2:L14">
@@ -7699,19 +7740,13 @@
       <formula>$G$24</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O22:O24 O26 O29:O36">
-    <cfRule type="cellIs" dxfId="10" priority="72" operator="between">
-      <formula>1</formula>
-      <formula>10</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="R2:R36">
-    <cfRule type="cellIs" dxfId="9" priority="71" operator="equal">
+  <conditionalFormatting sqref="R2:R37">
+    <cfRule type="cellIs" dxfId="10" priority="71" operator="equal">
       <formula>"NO"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R2:R36">
-    <cfRule type="cellIs" dxfId="8" priority="70" operator="equal">
+  <conditionalFormatting sqref="R2:R37">
+    <cfRule type="cellIs" dxfId="9" priority="70" operator="equal">
       <formula>"YES"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7838,14 +7873,8 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="107" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="8" priority="107" operator="greaterThan">
       <formula>$G$24</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O25">
-    <cfRule type="cellIs" dxfId="6" priority="45" operator="between">
-      <formula>1</formula>
-      <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q1:Q1048576">
@@ -7939,7 +7968,7 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="109" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="7" priority="109" operator="greaterThan">
       <formula>$G$24</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7953,12 +7982,6 @@
         <color rgb="FFFCFCFF"/>
         <color rgb="FF63BE7B"/>
       </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O27">
-    <cfRule type="cellIs" dxfId="4" priority="23" operator="between">
-      <formula>1</formula>
-      <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L28">
@@ -8028,7 +8051,7 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="19" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="6" priority="19" operator="greaterThan">
       <formula>$G$24</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8044,10 +8067,22 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O28">
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="between">
+  <conditionalFormatting sqref="O1:O1048576">
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="between">
       <formula>1</formula>
       <formula>10</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="23" operator="between">
+      <formula>10</formula>
+      <formula>20</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="45" operator="between">
+      <formula>21</formula>
+      <formula>30</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="72" operator="between">
+      <formula>31</formula>
+      <formula>50</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K37:K40">

</xml_diff>